<commit_message>
07.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Allocation Sheet.xlsx
+++ b/September/Others/Allocation Sheet.xlsx
@@ -887,6 +887,115 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -899,20 +1008,35 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -934,130 +1058,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1241,15 +1241,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>52280</xdr:rowOff>
+      <xdr:rowOff>42755</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>268466</xdr:colOff>
+      <xdr:colOff>277991</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>124112</xdr:rowOff>
+      <xdr:rowOff>114587</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1260,7 +1260,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="180975" y="11834705"/>
+          <a:off x="190500" y="11825180"/>
           <a:ext cx="6688316" cy="271857"/>
           <a:chOff x="253" y="249"/>
           <a:chExt cx="630" cy="292"/>
@@ -1459,7 +1459,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2559,7 +2559,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3005,7 +3005,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3076,7 +3076,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3150,7 +3150,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3221,7 +3221,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3883,8 +3883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="S54" sqref="S54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3906,50 +3906,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="47"/>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="46" t="s">
+      <c r="A1" s="76"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
     </row>
     <row r="3" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="72"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="39"/>
       <c r="F3" s="39"/>
       <c r="G3" s="39"/>
@@ -3957,14 +3957,14 @@
       <c r="I3" s="39"/>
       <c r="J3" s="39"/>
       <c r="K3" s="39"/>
-      <c r="L3" s="73" t="s">
+      <c r="L3" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="M3" s="74"/>
-      <c r="N3" s="71" t="s">
+      <c r="M3" s="72"/>
+      <c r="N3" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="O3" s="72"/>
+      <c r="O3" s="74"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickTop="1">
       <c r="A4" s="26" t="s">
@@ -4142,13 +4142,13 @@
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
-      <c r="I9" s="76" t="s">
+      <c r="I9" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="J9" s="77">
+      <c r="J9" s="45">
         <v>1100</v>
       </c>
-      <c r="K9" s="78">
+      <c r="K9" s="46">
         <v>1190</v>
       </c>
       <c r="L9" s="31"/>
@@ -5108,14 +5108,14 @@
       <c r="F43" s="31"/>
       <c r="G43" s="31"/>
       <c r="H43" s="31"/>
-      <c r="I43" s="44" t="s">
+      <c r="I43" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="J43" s="44"/>
+      <c r="J43" s="77"/>
       <c r="K43" s="31"/>
       <c r="L43" s="31"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44"/>
+      <c r="M43" s="77"/>
+      <c r="N43" s="77"/>
       <c r="O43" s="36"/>
     </row>
     <row r="44" spans="1:15" ht="17.100000000000001" customHeight="1">
@@ -5133,13 +5133,13 @@
       <c r="F44" s="31"/>
       <c r="G44" s="31"/>
       <c r="H44" s="31"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="44"/>
-      <c r="L44" s="44"/>
-      <c r="M44" s="44"/>
-      <c r="N44" s="44"/>
-      <c r="O44" s="44"/>
+      <c r="I44" s="77"/>
+      <c r="J44" s="77"/>
+      <c r="K44" s="77"/>
+      <c r="L44" s="77"/>
+      <c r="M44" s="77"/>
+      <c r="N44" s="77"/>
+      <c r="O44" s="77"/>
     </row>
     <row r="45" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="29" t="s">
@@ -5156,15 +5156,15 @@
       <c r="F45" s="31"/>
       <c r="G45" s="31"/>
       <c r="H45" s="31"/>
-      <c r="I45" s="40" t="s">
+      <c r="I45" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="J45" s="40"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="40"/>
-      <c r="N45" s="40"/>
-      <c r="O45" s="41"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="79"/>
+      <c r="M45" s="79"/>
+      <c r="N45" s="79"/>
+      <c r="O45" s="80"/>
     </row>
     <row r="46" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="29" t="s">
@@ -5187,13 +5187,13 @@
       <c r="J46" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="K46" s="44" t="s">
+      <c r="K46" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="L46" s="44"/>
-      <c r="M46" s="44"/>
-      <c r="N46" s="44"/>
-      <c r="O46" s="42"/>
+      <c r="L46" s="77"/>
+      <c r="M46" s="77"/>
+      <c r="N46" s="77"/>
+      <c r="O46" s="81"/>
     </row>
     <row r="47" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A47" s="29" t="s">
@@ -5218,7 +5218,7 @@
       <c r="L47" s="31"/>
       <c r="M47" s="31"/>
       <c r="N47" s="31"/>
-      <c r="O47" s="42"/>
+      <c r="O47" s="81"/>
     </row>
     <row r="48" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="29" t="s">
@@ -5243,7 +5243,7 @@
       <c r="L48" s="31"/>
       <c r="M48" s="31"/>
       <c r="N48" s="31"/>
-      <c r="O48" s="42"/>
+      <c r="O48" s="81"/>
     </row>
     <row r="49" spans="1:16" ht="17.100000000000001" customHeight="1">
       <c r="A49" s="31" t="s">
@@ -5268,7 +5268,7 @@
       <c r="L49" s="31"/>
       <c r="M49" s="31"/>
       <c r="N49" s="31"/>
-      <c r="O49" s="42"/>
+      <c r="O49" s="81"/>
     </row>
     <row r="50" spans="1:16" ht="17.100000000000001" customHeight="1">
       <c r="A50" s="31" t="s">
@@ -5293,7 +5293,7 @@
       <c r="L50" s="31"/>
       <c r="M50" s="31"/>
       <c r="N50" s="31"/>
-      <c r="O50" s="42"/>
+      <c r="O50" s="81"/>
     </row>
     <row r="51" spans="1:16" ht="17.100000000000001" customHeight="1">
       <c r="A51" s="31" t="s">
@@ -5318,7 +5318,7 @@
       <c r="L51" s="31"/>
       <c r="M51" s="31"/>
       <c r="N51" s="31"/>
-      <c r="O51" s="42"/>
+      <c r="O51" s="81"/>
     </row>
     <row r="52" spans="1:16" ht="17.100000000000001" customHeight="1">
       <c r="A52" s="31" t="s">
@@ -5343,7 +5343,7 @@
       <c r="L52" s="31"/>
       <c r="M52" s="31"/>
       <c r="N52" s="31"/>
-      <c r="O52" s="42"/>
+      <c r="O52" s="81"/>
     </row>
     <row r="53" spans="1:16" ht="17.100000000000001" customHeight="1">
       <c r="A53" s="31" t="s">
@@ -5368,7 +5368,7 @@
       <c r="L53" s="31"/>
       <c r="M53" s="31"/>
       <c r="N53" s="31"/>
-      <c r="O53" s="42"/>
+      <c r="O53" s="81"/>
     </row>
     <row r="54" spans="1:16" ht="17.100000000000001" customHeight="1">
       <c r="A54" s="31" t="s">
@@ -5393,7 +5393,7 @@
       <c r="L54" s="31"/>
       <c r="M54" s="31"/>
       <c r="N54" s="31"/>
-      <c r="O54" s="42"/>
+      <c r="O54" s="81"/>
     </row>
     <row r="55" spans="1:16" ht="17.100000000000001" customHeight="1">
       <c r="A55" s="29" t="s">
@@ -5408,9 +5408,9 @@
       <c r="D55" s="29"/>
       <c r="E55" s="29"/>
       <c r="F55" s="29"/>
-      <c r="G55" s="69"/>
-      <c r="H55" s="69"/>
-      <c r="I55" s="69" t="s">
+      <c r="G55" s="42"/>
+      <c r="H55" s="42"/>
+      <c r="I55" s="42" t="s">
         <v>12</v>
       </c>
       <c r="J55" s="31"/>
@@ -5418,122 +5418,110 @@
       <c r="L55" s="31"/>
       <c r="M55" s="31"/>
       <c r="N55" s="31"/>
-      <c r="O55" s="43"/>
+      <c r="O55" s="82"/>
     </row>
     <row r="56" spans="1:16">
-      <c r="A56" s="80" t="s">
+      <c r="A56" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="B56" s="81"/>
-      <c r="C56" s="81"/>
-      <c r="D56" s="82"/>
-      <c r="E56" s="83" t="s">
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="F56" s="83"/>
-      <c r="G56" s="83"/>
-      <c r="H56" s="83"/>
-      <c r="I56" s="83"/>
-      <c r="J56" s="83"/>
-      <c r="K56" s="83"/>
-      <c r="L56" s="82"/>
-      <c r="M56" s="84" t="s">
+      <c r="F56" s="56"/>
+      <c r="G56" s="56"/>
+      <c r="H56" s="56"/>
+      <c r="I56" s="56"/>
+      <c r="J56" s="56"/>
+      <c r="K56" s="56"/>
+      <c r="L56" s="48"/>
+      <c r="M56" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="N56" s="84"/>
-      <c r="O56" s="85"/>
+      <c r="N56" s="58"/>
+      <c r="O56" s="59"/>
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A57" s="86"/>
-      <c r="B57" s="87"/>
-      <c r="C57" s="87"/>
-      <c r="D57" s="88"/>
-      <c r="E57" s="89"/>
-      <c r="F57" s="89"/>
-      <c r="G57" s="89"/>
-      <c r="H57" s="89"/>
-      <c r="I57" s="89"/>
-      <c r="J57" s="89"/>
-      <c r="K57" s="89"/>
-      <c r="L57" s="88"/>
-      <c r="M57" s="90"/>
-      <c r="N57" s="90"/>
-      <c r="O57" s="91"/>
+      <c r="A57" s="54"/>
+      <c r="B57" s="55"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="49"/>
+      <c r="E57" s="57"/>
+      <c r="F57" s="57"/>
+      <c r="G57" s="57"/>
+      <c r="H57" s="57"/>
+      <c r="I57" s="57"/>
+      <c r="J57" s="57"/>
+      <c r="K57" s="57"/>
+      <c r="L57" s="49"/>
+      <c r="M57" s="60"/>
+      <c r="N57" s="60"/>
+      <c r="O57" s="61"/>
     </row>
     <row r="58" spans="1:16">
-      <c r="A58" s="66"/>
-      <c r="B58" s="66"/>
-      <c r="C58" s="66"/>
+      <c r="A58" s="40"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
       <c r="D58" s="37"/>
       <c r="E58" s="37"/>
       <c r="F58" s="37"/>
-      <c r="G58" s="66"/>
-      <c r="H58" s="66"/>
-      <c r="I58" s="66"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="40"/>
       <c r="J58" s="37"/>
       <c r="K58" s="37"/>
       <c r="L58" s="37"/>
       <c r="M58" s="37"/>
-      <c r="N58" s="67"/>
-      <c r="O58" s="67"/>
+      <c r="N58" s="41"/>
+      <c r="O58" s="41"/>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="96" t="s">
+      <c r="A59" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="96"/>
-      <c r="C59" s="96"/>
-      <c r="D59" s="95"/>
-      <c r="E59" s="66"/>
-      <c r="F59" s="66"/>
-      <c r="G59" s="92" t="s">
+      <c r="B59" s="62"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="51"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="H59" s="68"/>
-      <c r="I59" s="93"/>
-      <c r="J59" s="66"/>
-      <c r="K59" s="66"/>
-      <c r="L59" s="95"/>
-      <c r="M59" s="45" t="s">
+      <c r="H59" s="65"/>
+      <c r="I59" s="66"/>
+      <c r="J59" s="40"/>
+      <c r="K59" s="40"/>
+      <c r="L59" s="51"/>
+      <c r="M59" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="N59" s="45"/>
-      <c r="O59" s="45"/>
+      <c r="N59" s="63"/>
+      <c r="O59" s="63"/>
     </row>
     <row r="60" spans="1:16">
-      <c r="A60" s="94"/>
-      <c r="B60" s="94"/>
-      <c r="C60" s="94"/>
-      <c r="D60" s="95"/>
-      <c r="E60" s="66"/>
-      <c r="F60" s="66"/>
-      <c r="G60" s="97"/>
-      <c r="H60" s="98"/>
-      <c r="I60" s="99"/>
-      <c r="J60" s="66"/>
-      <c r="K60" s="66"/>
-      <c r="L60" s="95"/>
-      <c r="M60" s="66"/>
-      <c r="N60" s="66"/>
-      <c r="O60" s="66"/>
+      <c r="A60" s="50"/>
+      <c r="B60" s="50"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="51"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="67"/>
+      <c r="H60" s="68"/>
+      <c r="I60" s="69"/>
+      <c r="J60" s="40"/>
+      <c r="K60" s="40"/>
+      <c r="L60" s="51"/>
+      <c r="M60" s="40"/>
+      <c r="N60" s="40"/>
+      <c r="O60" s="40"/>
     </row>
     <row r="64" spans="1:16">
-      <c r="P64" s="79"/>
+      <c r="P64" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="E56:K57"/>
-    <mergeCell ref="M56:O57"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="M59:O59"/>
-    <mergeCell ref="G59:I60"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A1:E1"/>
     <mergeCell ref="I43:J43"/>
     <mergeCell ref="M43:N43"/>
     <mergeCell ref="A2:O2"/>
@@ -5541,6 +5529,18 @@
     <mergeCell ref="I45:N45"/>
     <mergeCell ref="O45:O55"/>
     <mergeCell ref="K46:N46"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="E56:K57"/>
+    <mergeCell ref="M56:O57"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="M59:O59"/>
+    <mergeCell ref="G59:I60"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.2" header="0" footer="0"/>
@@ -5577,73 +5577,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="95" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="53" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="97" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="51" t="s">
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="95" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="95"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5651,12 +5651,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="50" t="s">
+      <c r="L4" s="94" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="94"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
       <c r="A5" s="6" t="s">
@@ -6760,14 +6760,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="56" t="s">
+      <c r="I44" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="57"/>
+      <c r="J44" s="88"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="56"/>
-      <c r="N44" s="56"/>
+      <c r="M44" s="87"/>
+      <c r="N44" s="87"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -6785,13 +6785,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="56"/>
-      <c r="O45" s="56"/>
+      <c r="I45" s="87"/>
+      <c r="J45" s="87"/>
+      <c r="K45" s="87"/>
+      <c r="L45" s="87"/>
+      <c r="M45" s="87"/>
+      <c r="N45" s="87"/>
+      <c r="O45" s="87"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="9" t="s">
@@ -6808,15 +6808,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="58" t="s">
+      <c r="I46" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="58"/>
-      <c r="K46" s="58"/>
-      <c r="L46" s="58"/>
-      <c r="M46" s="58"/>
-      <c r="N46" s="58"/>
-      <c r="O46" s="59"/>
+      <c r="J46" s="89"/>
+      <c r="K46" s="89"/>
+      <c r="L46" s="89"/>
+      <c r="M46" s="89"/>
+      <c r="N46" s="89"/>
+      <c r="O46" s="90"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="9" t="s">
@@ -6839,13 +6839,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="56" t="s">
+      <c r="K47" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="56"/>
-      <c r="M47" s="56"/>
-      <c r="N47" s="56"/>
-      <c r="O47" s="60"/>
+      <c r="L47" s="87"/>
+      <c r="M47" s="87"/>
+      <c r="N47" s="87"/>
+      <c r="O47" s="91"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="9" t="s">
@@ -6870,7 +6870,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="60"/>
+      <c r="O48" s="91"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="9" t="s">
@@ -6895,7 +6895,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="60"/>
+      <c r="O49" s="91"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="4" t="s">
@@ -6920,7 +6920,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="60"/>
+      <c r="O50" s="91"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="4" t="s">
@@ -6945,7 +6945,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="60"/>
+      <c r="O51" s="91"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="4" t="s">
@@ -6970,7 +6970,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="60"/>
+      <c r="O52" s="91"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="4" t="s">
@@ -6995,7 +6995,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="60"/>
+      <c r="O53" s="91"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="4" t="s">
@@ -7020,7 +7020,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="60"/>
+      <c r="O54" s="91"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="4" t="s">
@@ -7045,7 +7045,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="60"/>
+      <c r="O55" s="91"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="9" t="s">
@@ -7070,7 +7070,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="61"/>
+      <c r="O56" s="92"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="17"/>
@@ -7090,49 +7090,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="62" t="s">
+      <c r="A58" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="62"/>
-      <c r="C58" s="62"/>
+      <c r="B58" s="83"/>
+      <c r="C58" s="83"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="65" t="s">
+      <c r="F58" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="65"/>
-      <c r="H58" s="65"/>
-      <c r="I58" s="65"/>
-      <c r="J58" s="65"/>
-      <c r="K58" s="65"/>
+      <c r="G58" s="86"/>
+      <c r="H58" s="86"/>
+      <c r="I58" s="86"/>
+      <c r="J58" s="86"/>
+      <c r="K58" s="86"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="63" t="s">
+      <c r="N58" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="63"/>
+      <c r="O58" s="84"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="64"/>
-      <c r="B59" s="64"/>
-      <c r="C59" s="64"/>
+      <c r="A59" s="85"/>
+      <c r="B59" s="85"/>
+      <c r="C59" s="85"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="65"/>
-      <c r="G59" s="65"/>
-      <c r="H59" s="65"/>
-      <c r="I59" s="65"/>
-      <c r="J59" s="65"/>
-      <c r="K59" s="65"/>
+      <c r="F59" s="86"/>
+      <c r="G59" s="86"/>
+      <c r="H59" s="86"/>
+      <c r="I59" s="86"/>
+      <c r="J59" s="86"/>
+      <c r="K59" s="86"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="64"/>
-      <c r="O59" s="64"/>
+      <c r="N59" s="85"/>
+      <c r="O59" s="85"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="64"/>
-      <c r="B60" s="64"/>
-      <c r="C60" s="64"/>
+      <c r="A60" s="85"/>
+      <c r="B60" s="85"/>
+      <c r="C60" s="85"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -7143,15 +7143,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="64"/>
-      <c r="O60" s="64"/>
+      <c r="N60" s="85"/>
+      <c r="O60" s="85"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="62" t="s">
+      <c r="A61" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="62"/>
-      <c r="C61" s="62"/>
+      <c r="B61" s="83"/>
+      <c r="C61" s="83"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -7162,11 +7162,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="63"/>
-      <c r="O61" s="63"/>
+      <c r="N61" s="84"/>
+      <c r="O61" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
     <mergeCell ref="A59:C60"/>
@@ -7174,19 +7187,6 @@
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="N61:O61"/>
     <mergeCell ref="F58:K59"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
10.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Allocation Sheet.xlsx
+++ b/September/Others/Allocation Sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="120">
   <si>
     <t>BL60</t>
   </si>
@@ -333,9 +333,6 @@
   </si>
   <si>
     <t>B65</t>
-  </si>
-  <si>
-    <t>Offer</t>
   </si>
   <si>
     <t>tulip2.rajshahi@gmail.com</t>
@@ -424,6 +421,18 @@
     <t xml:space="preserve">Total Qty = </t>
   </si>
   <si>
+    <t>L42</t>
+  </si>
+  <si>
+    <t>L130</t>
+  </si>
+  <si>
+    <t>S40</t>
+  </si>
+  <si>
+    <t>V99</t>
+  </si>
+  <si>
     <t>Md Robiul Islam</t>
   </si>
 </sst>
@@ -434,7 +443,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,23 +540,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -572,6 +564,40 @@
       <color rgb="FFFF0000"/>
       <name val="Berlin Sans FB Demi"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -780,7 +806,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -847,39 +873,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -890,23 +883,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -987,27 +968,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1057,6 +1023,63 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1241,13 +1264,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>147792</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>42755</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>277991</xdr:colOff>
+      <xdr:colOff>288667</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>114587</xdr:rowOff>
     </xdr:to>
@@ -1260,10 +1283,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="190500" y="11825180"/>
-          <a:ext cx="6688316" cy="271857"/>
-          <a:chOff x="253" y="249"/>
-          <a:chExt cx="630" cy="292"/>
+          <a:off x="147792" y="11825180"/>
+          <a:ext cx="6779800" cy="271857"/>
+          <a:chOff x="249" y="249"/>
+          <a:chExt cx="635" cy="292"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -1480,8 +1503,8 @@
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="862" y="279"/>
-            <a:ext cx="21" cy="258"/>
+            <a:off x="862" y="299"/>
+            <a:ext cx="22" cy="231"/>
           </a:xfrm>
           <a:custGeom>
             <a:avLst/>
@@ -2580,7 +2603,7 @@
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="253" y="285"/>
+            <a:off x="249" y="295"/>
             <a:ext cx="16" cy="205"/>
           </a:xfrm>
           <a:custGeom>
@@ -3883,1642 +3906,1635 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="S54" sqref="S54"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="38"/>
-    <col min="3" max="4" width="8.140625" style="38" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="38" customWidth="1"/>
-    <col min="6" max="6" width="9" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="38" customWidth="1"/>
-    <col min="8" max="8" width="1.85546875" style="38" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="38" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="38" customWidth="1"/>
-    <col min="11" max="12" width="7.140625" style="38" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="38" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="38" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" style="38" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="38"/>
+    <col min="1" max="1" width="9.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="27"/>
+    <col min="3" max="4" width="8.140625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="27" customWidth="1"/>
+    <col min="6" max="6" width="9" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="27" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" style="27" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="27" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="27" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" style="27" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" style="27" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="27" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="27" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="76"/>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="70" t="s">
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+    </row>
+    <row r="3" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A3" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="60"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="56" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-    </row>
-    <row r="3" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A3" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="71" t="s">
+      <c r="M3" s="57"/>
+      <c r="N3" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="O3" s="59"/>
+    </row>
+    <row r="4" spans="1:15" ht="16.5" thickTop="1">
+      <c r="A4" s="93" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="94" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="94"/>
+      <c r="I4" s="93" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="94" t="s">
+        <v>81</v>
+      </c>
+      <c r="L4" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="M4" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="94" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A5" s="97" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="81">
+        <v>800</v>
+      </c>
+      <c r="C5" s="82">
+        <v>875</v>
+      </c>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="96" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="83">
+        <v>5470</v>
+      </c>
+      <c r="K5" s="82">
+        <v>5890</v>
+      </c>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+    </row>
+    <row r="6" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A6" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="81">
+        <v>780</v>
+      </c>
+      <c r="C6" s="82">
+        <v>840</v>
+      </c>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="96" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="84">
+        <v>5750</v>
+      </c>
+      <c r="K6" s="82">
+        <v>6190</v>
+      </c>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+    </row>
+    <row r="7" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A7" s="97" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="81">
+        <v>865</v>
+      </c>
+      <c r="C7" s="82">
+        <v>925</v>
+      </c>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="97" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="80">
+        <v>5940</v>
+      </c>
+      <c r="K7" s="82">
+        <v>6390</v>
+      </c>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
+    </row>
+    <row r="8" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A8" s="97" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="81">
+        <v>810</v>
+      </c>
+      <c r="C8" s="82">
+        <v>880</v>
+      </c>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="97" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" s="83">
+        <v>6530</v>
+      </c>
+      <c r="K8" s="82">
+        <v>6990</v>
+      </c>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="82"/>
+    </row>
+    <row r="9" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A9" s="97" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="81">
+        <v>800</v>
+      </c>
+      <c r="C9" s="82">
+        <v>870</v>
+      </c>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="96" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" s="83">
+        <v>6890</v>
+      </c>
+      <c r="K9" s="82">
+        <v>7490</v>
+      </c>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="82"/>
+    </row>
+    <row r="10" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A10" s="97" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="81">
+        <v>795</v>
+      </c>
+      <c r="C10" s="82">
+        <v>865</v>
+      </c>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="96" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="83">
+        <v>8340</v>
+      </c>
+      <c r="K10" s="82">
+        <v>8990</v>
+      </c>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
+    </row>
+    <row r="11" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A11" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="81">
+        <v>790</v>
+      </c>
+      <c r="C11" s="82">
+        <v>860</v>
+      </c>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="97" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="83">
+        <v>9190</v>
+      </c>
+      <c r="K11" s="82">
+        <v>9990</v>
+      </c>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="82"/>
+      <c r="O11" s="82"/>
+    </row>
+    <row r="12" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A12" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="81">
+        <v>800</v>
+      </c>
+      <c r="C12" s="82">
+        <v>860</v>
+      </c>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="96" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="83">
+        <v>5750</v>
+      </c>
+      <c r="K12" s="82">
+        <v>6190</v>
+      </c>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="82"/>
+    </row>
+    <row r="13" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A13" s="97" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="81">
+        <v>790</v>
+      </c>
+      <c r="C13" s="82">
+        <v>850</v>
+      </c>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" s="83">
+        <v>4280</v>
+      </c>
+      <c r="K13" s="82">
+        <v>4590</v>
+      </c>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
+    </row>
+    <row r="14" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A14" s="97" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="81">
+        <v>970</v>
+      </c>
+      <c r="C14" s="82">
+        <v>1060</v>
+      </c>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="96" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="83">
+        <v>5650</v>
+      </c>
+      <c r="K14" s="82">
+        <v>6150</v>
+      </c>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+    </row>
+    <row r="15" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A15" s="97" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="81">
+        <v>900</v>
+      </c>
+      <c r="C15" s="82">
+        <v>975</v>
+      </c>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="96" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="83">
+        <v>5020</v>
+      </c>
+      <c r="K15" s="82">
+        <v>5390</v>
+      </c>
+      <c r="L15" s="82"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
+    </row>
+    <row r="16" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A16" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="81">
+        <v>915</v>
+      </c>
+      <c r="C16" s="82">
+        <v>990</v>
+      </c>
+      <c r="D16" s="82"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="82"/>
+      <c r="G16" s="82"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="97" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="83">
+        <v>5280</v>
+      </c>
+      <c r="K16" s="82">
+        <v>5690</v>
+      </c>
+      <c r="L16" s="82"/>
+      <c r="M16" s="82"/>
+      <c r="N16" s="82"/>
+      <c r="O16" s="82"/>
+    </row>
+    <row r="17" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A17" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="81">
+        <v>910</v>
+      </c>
+      <c r="C17" s="82">
+        <v>980</v>
+      </c>
+      <c r="D17" s="82"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" s="83">
+        <v>4550</v>
+      </c>
+      <c r="K17" s="82">
+        <v>4890</v>
+      </c>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="82"/>
+    </row>
+    <row r="18" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A18" s="97" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="81">
+        <v>890</v>
+      </c>
+      <c r="C18" s="82">
+        <v>970</v>
+      </c>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="83">
+        <v>5100</v>
+      </c>
+      <c r="K18" s="82">
+        <v>5490</v>
+      </c>
+      <c r="L18" s="82"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="82"/>
+      <c r="O18" s="82"/>
+    </row>
+    <row r="19" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A19" s="97" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="81">
+        <v>920</v>
+      </c>
+      <c r="C19" s="82">
+        <v>999</v>
+      </c>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="83">
+        <v>5560</v>
+      </c>
+      <c r="K19" s="82">
+        <v>5990</v>
+      </c>
+      <c r="L19" s="82"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="82"/>
+    </row>
+    <row r="20" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A20" s="97" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="81">
+        <v>880</v>
+      </c>
+      <c r="C20" s="82">
+        <v>950</v>
+      </c>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="97" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20" s="83">
+        <v>6090</v>
+      </c>
+      <c r="K20" s="82">
+        <v>6590</v>
+      </c>
+      <c r="L20" s="82"/>
+      <c r="M20" s="82"/>
+      <c r="N20" s="82"/>
+      <c r="O20" s="82"/>
+    </row>
+    <row r="21" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A21" s="97" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="81">
+        <v>845</v>
+      </c>
+      <c r="C21" s="82">
+        <v>910</v>
+      </c>
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="82"/>
+      <c r="H21" s="82"/>
+      <c r="I21" s="97" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="83">
+        <v>5390</v>
+      </c>
+      <c r="K21" s="82">
+        <v>5790</v>
+      </c>
+      <c r="L21" s="82"/>
+      <c r="M21" s="82"/>
+      <c r="N21" s="82"/>
+      <c r="O21" s="82"/>
+    </row>
+    <row r="22" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A22" s="97" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="81">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="82">
+        <v>1090</v>
+      </c>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="97" t="s">
+        <v>77</v>
+      </c>
+      <c r="J22" s="83">
+        <v>3630</v>
+      </c>
+      <c r="K22" s="82">
+        <v>3890</v>
+      </c>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="82"/>
+    </row>
+    <row r="23" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A23" s="97" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="81">
+        <v>995</v>
+      </c>
+      <c r="C23" s="82">
+        <v>1075</v>
+      </c>
+      <c r="D23" s="82"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="82"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="83">
+        <v>3560</v>
+      </c>
+      <c r="K23" s="82">
+        <v>3840</v>
+      </c>
+      <c r="L23" s="82"/>
+      <c r="M23" s="82"/>
+      <c r="N23" s="82"/>
+      <c r="O23" s="82"/>
+    </row>
+    <row r="24" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A24" s="97" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="81">
+        <v>880</v>
+      </c>
+      <c r="C24" s="82">
+        <v>950</v>
+      </c>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="97" t="s">
+        <v>78</v>
+      </c>
+      <c r="J24" s="83">
+        <v>3340</v>
+      </c>
+      <c r="K24" s="82">
+        <v>3590</v>
+      </c>
+      <c r="L24" s="82"/>
+      <c r="M24" s="82"/>
+      <c r="N24" s="82"/>
+      <c r="O24" s="82"/>
+    </row>
+    <row r="25" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A25" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="81">
+        <v>900</v>
+      </c>
+      <c r="C25" s="82">
+        <v>970</v>
+      </c>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="97" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" s="83">
+        <v>5390</v>
+      </c>
+      <c r="K25" s="82">
+        <v>5790</v>
+      </c>
+      <c r="L25" s="82"/>
+      <c r="M25" s="82"/>
+      <c r="N25" s="82"/>
+      <c r="O25" s="82"/>
+    </row>
+    <row r="26" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A26" s="97" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="81">
+        <v>1040</v>
+      </c>
+      <c r="C26" s="82">
+        <v>1120</v>
+      </c>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="82"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="97" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" s="83">
+        <v>4500</v>
+      </c>
+      <c r="K26" s="82">
+        <v>4790</v>
+      </c>
+      <c r="L26" s="82"/>
+      <c r="M26" s="82"/>
+      <c r="N26" s="82"/>
+      <c r="O26" s="82"/>
+    </row>
+    <row r="27" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A27" s="97" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="81">
+        <v>930</v>
+      </c>
+      <c r="C27" s="82">
+        <v>999</v>
+      </c>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="96" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="83">
+        <v>4970</v>
+      </c>
+      <c r="K27" s="82">
+        <v>5290</v>
+      </c>
+      <c r="L27" s="82"/>
+      <c r="M27" s="82"/>
+      <c r="N27" s="82"/>
+      <c r="O27" s="82"/>
+    </row>
+    <row r="28" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A28" s="97" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="81">
+        <v>1290</v>
+      </c>
+      <c r="C28" s="82">
+        <v>1390</v>
+      </c>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="J28" s="83">
+        <v>4015</v>
+      </c>
+      <c r="K28" s="82">
+        <v>4390</v>
+      </c>
+      <c r="L28" s="82"/>
+      <c r="M28" s="82"/>
+      <c r="N28" s="82"/>
+      <c r="O28" s="82"/>
+    </row>
+    <row r="29" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A29" s="97" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="81">
+        <v>1190</v>
+      </c>
+      <c r="C29" s="82">
+        <v>1290</v>
+      </c>
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="82"/>
+      <c r="I29" s="97" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29" s="84">
+        <v>3710</v>
+      </c>
+      <c r="K29" s="82">
+        <v>3990</v>
+      </c>
+      <c r="L29" s="82"/>
+      <c r="M29" s="82"/>
+      <c r="N29" s="82"/>
+      <c r="O29" s="82"/>
+    </row>
+    <row r="30" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A30" s="97" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="81">
+        <v>1270</v>
+      </c>
+      <c r="C30" s="82">
+        <v>1370</v>
+      </c>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="82"/>
+      <c r="I30" s="96" t="s">
+        <v>92</v>
+      </c>
+      <c r="J30" s="84">
+        <v>3620</v>
+      </c>
+      <c r="K30" s="82">
+        <v>3890</v>
+      </c>
+      <c r="L30" s="82"/>
+      <c r="M30" s="82"/>
+      <c r="N30" s="82"/>
+      <c r="O30" s="82"/>
+    </row>
+    <row r="31" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A31" s="97" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="81">
+        <v>1170</v>
+      </c>
+      <c r="C31" s="82">
+        <v>1270</v>
+      </c>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="82"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="96" t="s">
+        <v>13</v>
+      </c>
+      <c r="J31" s="84">
+        <v>4620</v>
+      </c>
+      <c r="K31" s="82">
+        <v>4999</v>
+      </c>
+      <c r="L31" s="82"/>
+      <c r="M31" s="82"/>
+      <c r="N31" s="82"/>
+      <c r="O31" s="82"/>
+    </row>
+    <row r="32" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A32" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="81">
+        <v>1190</v>
+      </c>
+      <c r="C32" s="82">
+        <v>1290</v>
+      </c>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="82"/>
+      <c r="I32" s="96" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" s="83">
+        <v>4520</v>
+      </c>
+      <c r="K32" s="82">
+        <v>4899</v>
+      </c>
+      <c r="L32" s="82"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="82"/>
+      <c r="O32" s="82"/>
+    </row>
+    <row r="33" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A33" s="97" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="81">
+        <v>1225</v>
+      </c>
+      <c r="C33" s="82">
+        <v>1325</v>
+      </c>
+      <c r="D33" s="82"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="82"/>
+      <c r="G33" s="82"/>
+      <c r="H33" s="82"/>
+      <c r="I33" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="J33" s="84">
+        <v>4080</v>
+      </c>
+      <c r="K33" s="82">
+        <v>4390</v>
+      </c>
+      <c r="L33" s="82"/>
+      <c r="M33" s="82"/>
+      <c r="N33" s="82"/>
+      <c r="O33" s="82"/>
+    </row>
+    <row r="34" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A34" s="97" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="81">
+        <v>1220</v>
+      </c>
+      <c r="C34" s="82">
+        <v>1320</v>
+      </c>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="82"/>
+      <c r="G34" s="82"/>
+      <c r="H34" s="82"/>
+      <c r="I34" s="97" t="s">
+        <v>93</v>
+      </c>
+      <c r="J34" s="83">
+        <v>4220</v>
+      </c>
+      <c r="K34" s="82">
+        <v>4540</v>
+      </c>
+      <c r="L34" s="82"/>
+      <c r="M34" s="82"/>
+      <c r="N34" s="82"/>
+      <c r="O34" s="82"/>
+    </row>
+    <row r="35" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A35" s="97" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="85">
+        <v>1080</v>
+      </c>
+      <c r="C35" s="82">
+        <v>1160</v>
+      </c>
+      <c r="D35" s="82"/>
+      <c r="E35" s="82"/>
+      <c r="F35" s="82"/>
+      <c r="G35" s="82"/>
+      <c r="H35" s="82"/>
+      <c r="I35" s="96" t="s">
+        <v>118</v>
+      </c>
+      <c r="J35" s="83"/>
+      <c r="K35" s="82"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="82"/>
+      <c r="N35" s="82"/>
+      <c r="O35" s="82"/>
+    </row>
+    <row r="36" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A36" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="81">
+        <v>1100</v>
+      </c>
+      <c r="C36" s="82">
+        <v>1199</v>
+      </c>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="96" t="s">
+        <v>55</v>
+      </c>
+      <c r="J36" s="83">
+        <v>12240</v>
+      </c>
+      <c r="K36" s="82">
+        <v>12990</v>
+      </c>
+      <c r="L36" s="82"/>
+      <c r="M36" s="82"/>
+      <c r="N36" s="82"/>
+      <c r="O36" s="82"/>
+    </row>
+    <row r="37" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A37" s="97" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="81">
+        <v>1200</v>
+      </c>
+      <c r="C37" s="82">
+        <v>1290</v>
+      </c>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="82"/>
+      <c r="I37" s="96" t="s">
+        <v>56</v>
+      </c>
+      <c r="J37" s="83">
+        <v>12090</v>
+      </c>
+      <c r="K37" s="82">
+        <v>12990</v>
+      </c>
+      <c r="L37" s="82"/>
+      <c r="M37" s="82"/>
+      <c r="N37" s="82"/>
+      <c r="O37" s="82"/>
+    </row>
+    <row r="38" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A38" s="97" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="81">
+        <v>1010</v>
+      </c>
+      <c r="C38" s="82">
+        <v>1110</v>
+      </c>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="82"/>
+      <c r="H38" s="82"/>
+      <c r="I38" s="96" t="s">
+        <v>57</v>
+      </c>
+      <c r="J38" s="83">
+        <v>10840</v>
+      </c>
+      <c r="K38" s="82">
+        <v>11990</v>
+      </c>
+      <c r="L38" s="82"/>
+      <c r="M38" s="82"/>
+      <c r="N38" s="82"/>
+      <c r="O38" s="82"/>
+    </row>
+    <row r="39" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A39" s="97" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="81">
+        <v>1040</v>
+      </c>
+      <c r="C39" s="82">
+        <v>1130</v>
+      </c>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="82"/>
+      <c r="H39" s="82"/>
+      <c r="I39" s="98" t="s">
+        <v>58</v>
+      </c>
+      <c r="J39" s="84">
+        <v>12490</v>
+      </c>
+      <c r="K39" s="82">
+        <v>13490</v>
+      </c>
+      <c r="L39" s="82"/>
+      <c r="M39" s="82"/>
+      <c r="N39" s="82"/>
+      <c r="O39" s="82"/>
+    </row>
+    <row r="40" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A40" s="97" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="81"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="82"/>
+      <c r="F40" s="82"/>
+      <c r="G40" s="82"/>
+      <c r="H40" s="82"/>
+      <c r="I40" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="J40" s="83">
+        <v>8820</v>
+      </c>
+      <c r="K40" s="82">
+        <v>9490</v>
+      </c>
+      <c r="L40" s="82"/>
+      <c r="M40" s="82"/>
+      <c r="N40" s="82"/>
+      <c r="O40" s="82"/>
+    </row>
+    <row r="41" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A41" s="97" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="81">
+        <v>1100</v>
+      </c>
+      <c r="C41" s="82">
+        <v>1199</v>
+      </c>
+      <c r="D41" s="82"/>
+      <c r="E41" s="82"/>
+      <c r="F41" s="82"/>
+      <c r="G41" s="82"/>
+      <c r="H41" s="82"/>
+      <c r="I41" s="96"/>
+      <c r="J41" s="83"/>
+      <c r="K41" s="82"/>
+      <c r="L41" s="82"/>
+      <c r="M41" s="82"/>
+      <c r="N41" s="82"/>
+      <c r="O41" s="82"/>
+    </row>
+    <row r="42" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A42" s="97" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="81">
+        <v>1100</v>
+      </c>
+      <c r="C42" s="82">
+        <v>1199</v>
+      </c>
+      <c r="D42" s="82"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="82"/>
+      <c r="G42" s="82"/>
+      <c r="H42" s="82"/>
+      <c r="I42" s="96"/>
+      <c r="J42" s="83"/>
+      <c r="K42" s="82"/>
+      <c r="L42" s="82"/>
+      <c r="M42" s="82"/>
+      <c r="N42" s="82"/>
+      <c r="O42" s="82"/>
+    </row>
+    <row r="43" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A43" s="97" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="81">
+        <v>1050</v>
+      </c>
+      <c r="C43" s="82">
+        <v>1130</v>
+      </c>
+      <c r="D43" s="82"/>
+      <c r="E43" s="82"/>
+      <c r="F43" s="82"/>
+      <c r="G43" s="82"/>
+      <c r="H43" s="82"/>
+      <c r="I43" s="86" t="s">
+        <v>12</v>
+      </c>
+      <c r="J43" s="86"/>
+      <c r="K43" s="82"/>
+      <c r="L43" s="82"/>
+      <c r="M43" s="86"/>
+      <c r="N43" s="86"/>
+      <c r="O43" s="87"/>
+    </row>
+    <row r="44" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A44" s="97" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="81">
+        <v>1130</v>
+      </c>
+      <c r="C44" s="82">
+        <v>1230</v>
+      </c>
+      <c r="D44" s="82"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="82"/>
+      <c r="G44" s="82"/>
+      <c r="H44" s="82"/>
+      <c r="I44" s="86"/>
+      <c r="J44" s="86"/>
+      <c r="K44" s="86"/>
+      <c r="L44" s="86"/>
+      <c r="M44" s="86"/>
+      <c r="N44" s="86"/>
+      <c r="O44" s="86"/>
+    </row>
+    <row r="45" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A45" s="97" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="81">
+        <v>1100</v>
+      </c>
+      <c r="C45" s="82">
+        <v>1190</v>
+      </c>
+      <c r="D45" s="82"/>
+      <c r="E45" s="82"/>
+      <c r="F45" s="82"/>
+      <c r="G45" s="82"/>
+      <c r="H45" s="82"/>
+      <c r="I45" s="88" t="s">
+        <v>8</v>
+      </c>
+      <c r="J45" s="88"/>
+      <c r="K45" s="88"/>
+      <c r="L45" s="88"/>
+      <c r="M45" s="88"/>
+      <c r="N45" s="88"/>
+      <c r="O45" s="89"/>
+    </row>
+    <row r="46" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A46" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="81">
+        <v>1330</v>
+      </c>
+      <c r="C46" s="82">
+        <v>1450</v>
+      </c>
+      <c r="D46" s="82"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="82"/>
+      <c r="G46" s="82"/>
+      <c r="H46" s="82"/>
+      <c r="I46" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="J46" s="84" t="s">
+        <v>9</v>
+      </c>
+      <c r="K46" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="L46" s="86"/>
+      <c r="M46" s="86"/>
+      <c r="N46" s="86"/>
+      <c r="O46" s="90"/>
+    </row>
+    <row r="47" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A47" s="97" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="81">
+        <v>1200</v>
+      </c>
+      <c r="C47" s="82">
+        <v>1299</v>
+      </c>
+      <c r="D47" s="82"/>
+      <c r="E47" s="82"/>
+      <c r="F47" s="82"/>
+      <c r="G47" s="82"/>
+      <c r="H47" s="82"/>
+      <c r="I47" s="82">
+        <v>1000</v>
+      </c>
+      <c r="J47" s="84"/>
+      <c r="K47" s="82"/>
+      <c r="L47" s="82"/>
+      <c r="M47" s="82"/>
+      <c r="N47" s="82"/>
+      <c r="O47" s="90"/>
+    </row>
+    <row r="48" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A48" s="97" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" s="81"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="82"/>
+      <c r="F48" s="82"/>
+      <c r="G48" s="82"/>
+      <c r="H48" s="82"/>
+      <c r="I48" s="82">
+        <v>500</v>
+      </c>
+      <c r="J48" s="84"/>
+      <c r="K48" s="82"/>
+      <c r="L48" s="82"/>
+      <c r="M48" s="82"/>
+      <c r="N48" s="82"/>
+      <c r="O48" s="90"/>
+    </row>
+    <row r="49" spans="1:16" ht="17.100000000000001" customHeight="1">
+      <c r="A49" s="98" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="82">
+        <v>1250</v>
+      </c>
+      <c r="C49" s="82">
+        <v>1350</v>
+      </c>
+      <c r="D49" s="82"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="82"/>
+      <c r="I49" s="82">
+        <v>100</v>
+      </c>
+      <c r="J49" s="84"/>
+      <c r="K49" s="82"/>
+      <c r="L49" s="82"/>
+      <c r="M49" s="82"/>
+      <c r="N49" s="82"/>
+      <c r="O49" s="90"/>
+    </row>
+    <row r="50" spans="1:16" ht="17.100000000000001" customHeight="1">
+      <c r="A50" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="82">
+        <v>1370</v>
+      </c>
+      <c r="C50" s="82">
+        <v>1490</v>
+      </c>
+      <c r="D50" s="82"/>
+      <c r="E50" s="82"/>
+      <c r="F50" s="82"/>
+      <c r="G50" s="82"/>
+      <c r="H50" s="82"/>
+      <c r="I50" s="82">
+        <v>50</v>
+      </c>
+      <c r="J50" s="84"/>
+      <c r="K50" s="82"/>
+      <c r="L50" s="82"/>
+      <c r="M50" s="82"/>
+      <c r="N50" s="82"/>
+      <c r="O50" s="90"/>
+    </row>
+    <row r="51" spans="1:16" ht="17.100000000000001" customHeight="1">
+      <c r="A51" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" s="82"/>
+      <c r="C51" s="82"/>
+      <c r="D51" s="82"/>
+      <c r="E51" s="82"/>
+      <c r="F51" s="82"/>
+      <c r="G51" s="82"/>
+      <c r="H51" s="82"/>
+      <c r="I51" s="82">
+        <v>20</v>
+      </c>
+      <c r="J51" s="84"/>
+      <c r="K51" s="82"/>
+      <c r="L51" s="82"/>
+      <c r="M51" s="82"/>
+      <c r="N51" s="82"/>
+      <c r="O51" s="90"/>
+    </row>
+    <row r="52" spans="1:16" ht="17.100000000000001" customHeight="1">
+      <c r="A52" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="M3" s="72"/>
-      <c r="N3" s="73" t="s">
-        <v>116</v>
-      </c>
-      <c r="O3" s="74"/>
-    </row>
-    <row r="4" spans="1:15" ht="16.5" thickTop="1">
-      <c r="A4" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="27" t="s">
+      <c r="B52" s="82">
+        <v>1100</v>
+      </c>
+      <c r="C52" s="82">
+        <v>1190</v>
+      </c>
+      <c r="D52" s="82"/>
+      <c r="E52" s="82"/>
+      <c r="F52" s="82"/>
+      <c r="G52" s="82"/>
+      <c r="H52" s="82"/>
+      <c r="I52" s="82">
+        <v>10</v>
+      </c>
+      <c r="J52" s="84"/>
+      <c r="K52" s="82"/>
+      <c r="L52" s="82"/>
+      <c r="M52" s="82"/>
+      <c r="N52" s="82"/>
+      <c r="O52" s="90"/>
+    </row>
+    <row r="53" spans="1:16" ht="17.100000000000001" customHeight="1">
+      <c r="A53" s="98" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="82">
+        <v>2780</v>
+      </c>
+      <c r="C53" s="82">
+        <v>2990</v>
+      </c>
+      <c r="D53" s="82"/>
+      <c r="E53" s="82"/>
+      <c r="F53" s="82"/>
+      <c r="G53" s="82"/>
+      <c r="H53" s="82"/>
+      <c r="I53" s="82">
         <v>5</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" s="27"/>
-      <c r="I4" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="L4" s="27" t="s">
+      <c r="J53" s="84"/>
+      <c r="K53" s="82"/>
+      <c r="L53" s="82"/>
+      <c r="M53" s="82"/>
+      <c r="N53" s="82"/>
+      <c r="O53" s="90"/>
+    </row>
+    <row r="54" spans="1:16" ht="17.100000000000001" customHeight="1">
+      <c r="A54" s="98" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="82">
+        <v>6540</v>
+      </c>
+      <c r="C54" s="82">
+        <v>6990</v>
+      </c>
+      <c r="D54" s="82"/>
+      <c r="E54" s="82"/>
+      <c r="F54" s="82"/>
+      <c r="G54" s="82"/>
+      <c r="H54" s="82"/>
+      <c r="I54" s="82">
+        <v>2</v>
+      </c>
+      <c r="J54" s="84"/>
+      <c r="K54" s="82"/>
+      <c r="L54" s="82"/>
+      <c r="M54" s="82"/>
+      <c r="N54" s="82"/>
+      <c r="O54" s="90"/>
+    </row>
+    <row r="55" spans="1:16" ht="17.100000000000001" customHeight="1">
+      <c r="A55" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" s="80">
+        <v>5290</v>
+      </c>
+      <c r="C55" s="80">
+        <v>5690</v>
+      </c>
+      <c r="D55" s="80"/>
+      <c r="E55" s="80"/>
+      <c r="F55" s="80"/>
+      <c r="G55" s="91"/>
+      <c r="H55" s="91"/>
+      <c r="I55" s="91" t="s">
+        <v>12</v>
+      </c>
+      <c r="J55" s="82"/>
+      <c r="K55" s="82"/>
+      <c r="L55" s="82"/>
+      <c r="M55" s="82"/>
+      <c r="N55" s="82"/>
+      <c r="O55" s="92"/>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="41"/>
+      <c r="K56" s="41"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="M4" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="N4" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="O4" s="27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A5" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="30">
-        <v>800</v>
-      </c>
-      <c r="C5" s="31">
-        <v>875</v>
-      </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="J5" s="32">
-        <v>6890</v>
-      </c>
-      <c r="K5" s="31">
-        <v>7490</v>
-      </c>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-    </row>
-    <row r="6" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A6" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="30">
-        <v>780</v>
-      </c>
-      <c r="C6" s="31">
-        <v>840</v>
-      </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="J6" s="34">
-        <v>8340</v>
-      </c>
-      <c r="K6" s="31">
-        <v>8990</v>
-      </c>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-    </row>
-    <row r="7" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A7" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="30">
-        <v>865</v>
-      </c>
-      <c r="C7" s="31">
-        <v>925</v>
-      </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="29">
-        <v>9190</v>
-      </c>
-      <c r="K7" s="31">
-        <v>9990</v>
-      </c>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-    </row>
-    <row r="8" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A8" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="30">
-        <v>810</v>
-      </c>
-      <c r="C8" s="31">
-        <v>880</v>
-      </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" s="32">
-        <v>5750</v>
-      </c>
-      <c r="K8" s="31">
-        <v>6190</v>
-      </c>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-    </row>
-    <row r="9" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A9" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="30">
-        <v>800</v>
-      </c>
-      <c r="C9" s="31">
-        <v>870</v>
-      </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="44" t="s">
+      <c r="N56" s="43"/>
+      <c r="O56" s="44"/>
+    </row>
+    <row r="57" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A57" s="39"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="42"/>
+      <c r="I57" s="42"/>
+      <c r="J57" s="42"/>
+      <c r="K57" s="42"/>
+      <c r="L57" s="34"/>
+      <c r="M57" s="45"/>
+      <c r="N57" s="45"/>
+      <c r="O57" s="46"/>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58" s="29"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="29"/>
+      <c r="H58" s="29"/>
+      <c r="I58" s="29"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="26"/>
+      <c r="L58" s="26"/>
+      <c r="M58" s="26"/>
+      <c r="N58" s="30"/>
+      <c r="O58" s="30"/>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="J9" s="45">
-        <v>1100</v>
-      </c>
-      <c r="K9" s="46">
-        <v>1190</v>
-      </c>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-    </row>
-    <row r="10" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A10" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="30">
-        <v>795</v>
-      </c>
-      <c r="C10" s="31">
-        <v>865</v>
-      </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="J10" s="32">
-        <v>4280</v>
-      </c>
-      <c r="K10" s="31">
-        <v>4590</v>
-      </c>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-    </row>
-    <row r="11" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A11" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="30">
-        <v>790</v>
-      </c>
-      <c r="C11" s="31">
-        <v>860</v>
-      </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="32">
-        <v>5650</v>
-      </c>
-      <c r="K11" s="31">
-        <v>6150</v>
-      </c>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-    </row>
-    <row r="12" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A12" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" s="30">
-        <v>800</v>
-      </c>
-      <c r="C12" s="31">
-        <v>860</v>
-      </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="32">
-        <v>5020</v>
-      </c>
-      <c r="K12" s="31">
-        <v>5390</v>
-      </c>
-      <c r="L12" s="31">
-        <v>400</v>
-      </c>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-    </row>
-    <row r="13" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A13" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="B13" s="30">
-        <v>790</v>
-      </c>
-      <c r="C13" s="31">
-        <v>850</v>
-      </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="32">
-        <v>5280</v>
-      </c>
-      <c r="K13" s="31">
-        <v>5690</v>
-      </c>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-    </row>
-    <row r="14" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A14" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="30">
-        <v>970</v>
-      </c>
-      <c r="C14" s="31">
-        <v>1060</v>
-      </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J14" s="32">
-        <v>4550</v>
-      </c>
-      <c r="K14" s="31">
-        <v>4890</v>
-      </c>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-    </row>
-    <row r="15" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A15" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="30">
-        <v>900</v>
-      </c>
-      <c r="C15" s="31">
-        <v>975</v>
-      </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="J15" s="32">
-        <v>5100</v>
-      </c>
-      <c r="K15" s="31">
-        <v>5490</v>
-      </c>
-      <c r="L15" s="31">
-        <v>70</v>
-      </c>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-    </row>
-    <row r="16" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A16" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="30">
-        <v>915</v>
-      </c>
-      <c r="C16" s="31">
-        <v>990</v>
-      </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="J16" s="32">
-        <v>5560</v>
-      </c>
-      <c r="K16" s="31">
-        <v>5990</v>
-      </c>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-    </row>
-    <row r="17" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A17" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="30">
-        <v>910</v>
-      </c>
-      <c r="C17" s="31">
-        <v>980</v>
-      </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="J17" s="32">
-        <v>6090</v>
-      </c>
-      <c r="K17" s="31">
-        <v>6590</v>
-      </c>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-    </row>
-    <row r="18" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A18" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="30">
-        <v>890</v>
-      </c>
-      <c r="C18" s="31">
-        <v>970</v>
-      </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="J18" s="32">
-        <v>5390</v>
-      </c>
-      <c r="K18" s="31">
-        <v>5790</v>
-      </c>
-      <c r="L18" s="31">
-        <v>200</v>
-      </c>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-    </row>
-    <row r="19" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A19" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="30">
-        <v>920</v>
-      </c>
-      <c r="C19" s="31">
-        <v>999</v>
-      </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="J19" s="32">
-        <v>3630</v>
-      </c>
-      <c r="K19" s="31">
-        <v>3890</v>
-      </c>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-    </row>
-    <row r="20" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A20" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="30">
-        <v>880</v>
-      </c>
-      <c r="C20" s="31">
-        <v>950</v>
-      </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="J20" s="32">
-        <v>3560</v>
-      </c>
-      <c r="K20" s="31">
-        <v>3840</v>
-      </c>
-      <c r="L20" s="31">
-        <v>400</v>
-      </c>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
-    </row>
-    <row r="21" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A21" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="30">
-        <v>845</v>
-      </c>
-      <c r="C21" s="31">
-        <v>910</v>
-      </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="J21" s="32">
-        <v>3340</v>
-      </c>
-      <c r="K21" s="31">
-        <v>3590</v>
-      </c>
-      <c r="L21" s="31">
-        <v>320</v>
-      </c>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
-    </row>
-    <row r="22" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A22" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="30">
-        <v>1000</v>
-      </c>
-      <c r="C22" s="31">
-        <v>1090</v>
-      </c>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="32">
-        <v>5390</v>
-      </c>
-      <c r="K22" s="31">
-        <v>5790</v>
-      </c>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-    </row>
-    <row r="23" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A23" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="30">
-        <v>995</v>
-      </c>
-      <c r="C23" s="31">
-        <v>1075</v>
-      </c>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="J23" s="32">
-        <v>4500</v>
-      </c>
-      <c r="K23" s="31">
-        <v>4790</v>
-      </c>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-    </row>
-    <row r="24" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A24" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="30">
-        <v>880</v>
-      </c>
-      <c r="C24" s="31">
-        <v>950</v>
-      </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" s="32">
-        <v>4970</v>
-      </c>
-      <c r="K24" s="31">
-        <v>5290</v>
-      </c>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-    </row>
-    <row r="25" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A25" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="30">
-        <v>900</v>
-      </c>
-      <c r="C25" s="31">
-        <v>970</v>
-      </c>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="J25" s="32">
-        <v>4015</v>
-      </c>
-      <c r="K25" s="31">
-        <v>4390</v>
-      </c>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-    </row>
-    <row r="26" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A26" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="30">
-        <v>1040</v>
-      </c>
-      <c r="C26" s="31">
-        <v>1120</v>
-      </c>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="J26" s="32">
-        <v>3710</v>
-      </c>
-      <c r="K26" s="31">
-        <v>3990</v>
-      </c>
-      <c r="L26" s="31">
-        <v>200</v>
-      </c>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-    </row>
-    <row r="27" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A27" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="30">
-        <v>930</v>
-      </c>
-      <c r="C27" s="31">
-        <v>999</v>
-      </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="J27" s="32">
-        <v>3620</v>
-      </c>
-      <c r="K27" s="31">
-        <v>3890</v>
-      </c>
-      <c r="L27" s="31">
-        <v>320</v>
-      </c>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-    </row>
-    <row r="28" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A28" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" s="30">
-        <v>1290</v>
-      </c>
-      <c r="C28" s="31">
-        <v>1390</v>
-      </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="J28" s="32">
-        <v>4620</v>
-      </c>
-      <c r="K28" s="31">
-        <v>4999</v>
-      </c>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-    </row>
-    <row r="29" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A29" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29" s="30">
-        <v>1190</v>
-      </c>
-      <c r="C29" s="31">
-        <v>1290</v>
-      </c>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="J29" s="34">
-        <v>4520</v>
-      </c>
-      <c r="K29" s="31">
-        <v>4899</v>
-      </c>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-    </row>
-    <row r="30" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A30" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="30">
-        <v>1270</v>
-      </c>
-      <c r="C30" s="31">
-        <v>1370</v>
-      </c>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="J30" s="34">
-        <v>4080</v>
-      </c>
-      <c r="K30" s="31">
-        <v>4390</v>
-      </c>
-      <c r="L30" s="31">
-        <v>200</v>
-      </c>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-    </row>
-    <row r="31" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A31" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="30">
-        <v>1170</v>
-      </c>
-      <c r="C31" s="31">
-        <v>1270</v>
-      </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="J31" s="34">
-        <v>4220</v>
-      </c>
-      <c r="K31" s="31">
-        <v>4540</v>
-      </c>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
-    </row>
-    <row r="32" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A32" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="30">
-        <v>1190</v>
-      </c>
-      <c r="C32" s="31">
-        <v>1290</v>
-      </c>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="J32" s="32">
-        <v>12240</v>
-      </c>
-      <c r="K32" s="31">
-        <v>12990</v>
-      </c>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-    </row>
-    <row r="33" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A33" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="30">
-        <v>1225</v>
-      </c>
-      <c r="C33" s="31">
-        <v>1325</v>
-      </c>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="J33" s="34">
-        <v>12090</v>
-      </c>
-      <c r="K33" s="31">
-        <v>12990</v>
-      </c>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
-    </row>
-    <row r="34" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A34" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="30">
-        <v>1220</v>
-      </c>
-      <c r="C34" s="31">
-        <v>1320</v>
-      </c>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="J34" s="32">
-        <v>10840</v>
-      </c>
-      <c r="K34" s="31">
-        <v>11990</v>
-      </c>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
-    </row>
-    <row r="35" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A35" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="35">
-        <v>1080</v>
-      </c>
-      <c r="C35" s="31">
-        <v>1160</v>
-      </c>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="J35" s="32">
-        <v>12490</v>
-      </c>
-      <c r="K35" s="31">
-        <v>13490</v>
-      </c>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="31"/>
-      <c r="O35" s="31"/>
-    </row>
-    <row r="36" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A36" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" s="30">
-        <v>1100</v>
-      </c>
-      <c r="C36" s="31">
-        <v>1199</v>
-      </c>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="J36" s="32">
-        <v>8820</v>
-      </c>
-      <c r="K36" s="31">
-        <v>9490</v>
-      </c>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="31"/>
-    </row>
-    <row r="37" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A37" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" s="30">
-        <v>1200</v>
-      </c>
-      <c r="C37" s="31">
-        <v>1290</v>
-      </c>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="31"/>
-      <c r="L37" s="31"/>
-      <c r="M37" s="31"/>
-      <c r="N37" s="31"/>
-      <c r="O37" s="31"/>
-    </row>
-    <row r="38" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A38" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="30">
-        <v>1010</v>
-      </c>
-      <c r="C38" s="31">
-        <v>1110</v>
-      </c>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="31"/>
-      <c r="L38" s="31"/>
-      <c r="M38" s="31"/>
-      <c r="N38" s="31"/>
-      <c r="O38" s="31"/>
-    </row>
-    <row r="39" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A39" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="30">
-        <v>1040</v>
-      </c>
-      <c r="C39" s="31">
-        <v>1130</v>
-      </c>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="31"/>
-      <c r="L39" s="31"/>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
-    </row>
-    <row r="40" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A40" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="30">
-        <v>1100</v>
-      </c>
-      <c r="C40" s="31">
-        <v>1199</v>
-      </c>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="31"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="31"/>
-    </row>
-    <row r="41" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A41" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="30">
-        <v>1100</v>
-      </c>
-      <c r="C41" s="31">
-        <v>1199</v>
-      </c>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="33"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31"/>
-    </row>
-    <row r="42" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A42" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="30">
-        <v>1050</v>
-      </c>
-      <c r="C42" s="31">
-        <v>1130</v>
-      </c>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="33"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="31"/>
-      <c r="M42" s="31"/>
-      <c r="N42" s="31"/>
-      <c r="O42" s="31"/>
-    </row>
-    <row r="43" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A43" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="30">
-        <v>1130</v>
-      </c>
-      <c r="C43" s="31">
-        <v>1230</v>
-      </c>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="77" t="s">
-        <v>12</v>
-      </c>
-      <c r="J43" s="77"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="77"/>
-      <c r="N43" s="77"/>
-      <c r="O43" s="36"/>
-    </row>
-    <row r="44" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A44" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" s="30">
-        <v>1100</v>
-      </c>
-      <c r="C44" s="31">
-        <v>1190</v>
-      </c>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="77"/>
-      <c r="J44" s="77"/>
-      <c r="K44" s="77"/>
-      <c r="L44" s="77"/>
-      <c r="M44" s="77"/>
-      <c r="N44" s="77"/>
-      <c r="O44" s="77"/>
-    </row>
-    <row r="45" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A45" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" s="30">
-        <v>1330</v>
-      </c>
-      <c r="C45" s="31">
-        <v>1450</v>
-      </c>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="79" t="s">
-        <v>8</v>
-      </c>
-      <c r="J45" s="79"/>
-      <c r="K45" s="79"/>
-      <c r="L45" s="79"/>
-      <c r="M45" s="79"/>
-      <c r="N45" s="79"/>
-      <c r="O45" s="80"/>
-    </row>
-    <row r="46" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A46" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46" s="30">
-        <v>1200</v>
-      </c>
-      <c r="C46" s="31">
-        <v>1299</v>
-      </c>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="J46" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="K46" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="L46" s="77"/>
-      <c r="M46" s="77"/>
-      <c r="N46" s="77"/>
-      <c r="O46" s="81"/>
-    </row>
-    <row r="47" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A47" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B47" s="30">
-        <v>1250</v>
-      </c>
-      <c r="C47" s="31">
-        <v>1350</v>
-      </c>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="31">
-        <v>1000</v>
-      </c>
-      <c r="J47" s="34"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="31"/>
-      <c r="M47" s="31"/>
-      <c r="N47" s="31"/>
-      <c r="O47" s="81"/>
-    </row>
-    <row r="48" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A48" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="30">
-        <v>1370</v>
-      </c>
-      <c r="C48" s="31">
-        <v>1490</v>
-      </c>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="31"/>
-      <c r="I48" s="31">
-        <v>500</v>
-      </c>
-      <c r="J48" s="34"/>
-      <c r="K48" s="31"/>
-      <c r="L48" s="31"/>
-      <c r="M48" s="31"/>
-      <c r="N48" s="31"/>
-      <c r="O48" s="81"/>
-    </row>
-    <row r="49" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A49" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="31">
-        <v>2780</v>
-      </c>
-      <c r="C49" s="31">
-        <v>2990</v>
-      </c>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="31">
-        <v>100</v>
-      </c>
-      <c r="J49" s="34"/>
-      <c r="K49" s="31"/>
-      <c r="L49" s="31"/>
-      <c r="M49" s="31"/>
-      <c r="N49" s="31"/>
-      <c r="O49" s="81"/>
-    </row>
-    <row r="50" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A50" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="31">
-        <v>6540</v>
-      </c>
-      <c r="C50" s="31">
-        <v>6990</v>
-      </c>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31">
-        <v>50</v>
-      </c>
-      <c r="J50" s="34"/>
-      <c r="K50" s="31"/>
-      <c r="L50" s="31"/>
-      <c r="M50" s="31"/>
-      <c r="N50" s="31"/>
-      <c r="O50" s="81"/>
-    </row>
-    <row r="51" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A51" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="31">
-        <v>5290</v>
-      </c>
-      <c r="C51" s="31">
-        <v>5690</v>
-      </c>
-      <c r="D51" s="31"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="31">
-        <v>20</v>
-      </c>
-      <c r="J51" s="34"/>
-      <c r="K51" s="31"/>
-      <c r="L51" s="31"/>
-      <c r="M51" s="31"/>
-      <c r="N51" s="31"/>
-      <c r="O51" s="81"/>
-    </row>
-    <row r="52" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A52" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="B52" s="31">
-        <v>5470</v>
-      </c>
-      <c r="C52" s="31">
-        <v>5890</v>
-      </c>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
-      <c r="H52" s="31"/>
-      <c r="I52" s="31">
-        <v>10</v>
-      </c>
-      <c r="J52" s="34"/>
-      <c r="K52" s="31"/>
-      <c r="L52" s="31"/>
-      <c r="M52" s="31"/>
-      <c r="N52" s="31"/>
-      <c r="O52" s="81"/>
-    </row>
-    <row r="53" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A53" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="B53" s="31">
-        <v>5750</v>
-      </c>
-      <c r="C53" s="31">
-        <v>6190</v>
-      </c>
-      <c r="D53" s="31"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="31"/>
-      <c r="H53" s="31"/>
-      <c r="I53" s="31">
-        <v>5</v>
-      </c>
-      <c r="J53" s="34"/>
-      <c r="K53" s="31"/>
-      <c r="L53" s="31"/>
-      <c r="M53" s="31"/>
-      <c r="N53" s="31"/>
-      <c r="O53" s="81"/>
-    </row>
-    <row r="54" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A54" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="B54" s="31">
-        <v>5940</v>
-      </c>
-      <c r="C54" s="31">
-        <v>6390</v>
-      </c>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="31">
-        <v>2</v>
-      </c>
-      <c r="J54" s="34"/>
-      <c r="K54" s="31"/>
-      <c r="L54" s="31"/>
-      <c r="M54" s="31"/>
-      <c r="N54" s="31"/>
-      <c r="O54" s="81"/>
-    </row>
-    <row r="55" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A55" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55" s="29">
-        <v>6530</v>
-      </c>
-      <c r="C55" s="29">
-        <v>6990</v>
-      </c>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="42"/>
-      <c r="H55" s="42"/>
-      <c r="I55" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="J55" s="31"/>
-      <c r="K55" s="31"/>
-      <c r="L55" s="31"/>
-      <c r="M55" s="31"/>
-      <c r="N55" s="31"/>
-      <c r="O55" s="82"/>
-    </row>
-    <row r="56" spans="1:16">
-      <c r="A56" s="52" t="s">
-        <v>108</v>
-      </c>
-      <c r="B56" s="53"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="48"/>
-      <c r="E56" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="F56" s="56"/>
-      <c r="G56" s="56"/>
-      <c r="H56" s="56"/>
-      <c r="I56" s="56"/>
-      <c r="J56" s="56"/>
-      <c r="K56" s="56"/>
-      <c r="L56" s="48"/>
-      <c r="M56" s="58" t="s">
-        <v>107</v>
-      </c>
-      <c r="N56" s="58"/>
-      <c r="O56" s="59"/>
-    </row>
-    <row r="57" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A57" s="54"/>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="57"/>
-      <c r="F57" s="57"/>
-      <c r="G57" s="57"/>
-      <c r="H57" s="57"/>
-      <c r="I57" s="57"/>
-      <c r="J57" s="57"/>
-      <c r="K57" s="57"/>
-      <c r="L57" s="49"/>
-      <c r="M57" s="60"/>
-      <c r="N57" s="60"/>
-      <c r="O57" s="61"/>
-    </row>
-    <row r="58" spans="1:16">
-      <c r="A58" s="40"/>
-      <c r="B58" s="40"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="37"/>
-      <c r="L58" s="37"/>
-      <c r="M58" s="37"/>
-      <c r="N58" s="41"/>
-      <c r="O58" s="41"/>
-    </row>
-    <row r="59" spans="1:16">
-      <c r="A59" s="62" t="s">
+      <c r="B59" s="47"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="H59" s="50"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="29"/>
+      <c r="K59" s="29"/>
+      <c r="L59" s="36"/>
+      <c r="M59" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="62"/>
-      <c r="C59" s="62"/>
-      <c r="D59" s="51"/>
-      <c r="E59" s="40"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="H59" s="65"/>
-      <c r="I59" s="66"/>
-      <c r="J59" s="40"/>
-      <c r="K59" s="40"/>
-      <c r="L59" s="51"/>
-      <c r="M59" s="63" t="s">
-        <v>114</v>
-      </c>
-      <c r="N59" s="63"/>
-      <c r="O59" s="63"/>
+      <c r="N59" s="48"/>
+      <c r="O59" s="48"/>
     </row>
     <row r="60" spans="1:16">
-      <c r="A60" s="50"/>
-      <c r="B60" s="50"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="51"/>
-      <c r="E60" s="40"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="67"/>
-      <c r="H60" s="68"/>
-      <c r="I60" s="69"/>
-      <c r="J60" s="40"/>
-      <c r="K60" s="40"/>
-      <c r="L60" s="51"/>
-      <c r="M60" s="40"/>
-      <c r="N60" s="40"/>
-      <c r="O60" s="40"/>
+      <c r="A60" s="35"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="52"/>
+      <c r="H60" s="53"/>
+      <c r="I60" s="54"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="36"/>
+      <c r="M60" s="29"/>
+      <c r="N60" s="29"/>
+      <c r="O60" s="29"/>
     </row>
     <row r="64" spans="1:16">
-      <c r="P64" s="47"/>
+      <c r="P64" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -5577,73 +5593,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="97" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="95" t="s">
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5651,12 +5667,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="94" t="s">
+      <c r="L4" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="94"/>
-      <c r="N4" s="94"/>
-      <c r="O4" s="94"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="74"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
       <c r="A5" s="6" t="s">
@@ -6760,14 +6776,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="87" t="s">
+      <c r="I44" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="88"/>
+      <c r="J44" s="68"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="87"/>
-      <c r="N44" s="87"/>
+      <c r="M44" s="67"/>
+      <c r="N44" s="67"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -6785,13 +6801,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="87"/>
-      <c r="J45" s="87"/>
-      <c r="K45" s="87"/>
-      <c r="L45" s="87"/>
-      <c r="M45" s="87"/>
-      <c r="N45" s="87"/>
-      <c r="O45" s="87"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="67"/>
+      <c r="L45" s="67"/>
+      <c r="M45" s="67"/>
+      <c r="N45" s="67"/>
+      <c r="O45" s="67"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="9" t="s">
@@ -6808,15 +6824,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="89" t="s">
+      <c r="I46" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="89"/>
-      <c r="K46" s="89"/>
-      <c r="L46" s="89"/>
-      <c r="M46" s="89"/>
-      <c r="N46" s="89"/>
-      <c r="O46" s="90"/>
+      <c r="J46" s="69"/>
+      <c r="K46" s="69"/>
+      <c r="L46" s="69"/>
+      <c r="M46" s="69"/>
+      <c r="N46" s="69"/>
+      <c r="O46" s="70"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="9" t="s">
@@ -6839,13 +6855,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="87" t="s">
+      <c r="K47" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="87"/>
-      <c r="M47" s="87"/>
-      <c r="N47" s="87"/>
-      <c r="O47" s="91"/>
+      <c r="L47" s="67"/>
+      <c r="M47" s="67"/>
+      <c r="N47" s="67"/>
+      <c r="O47" s="71"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="9" t="s">
@@ -6870,7 +6886,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="91"/>
+      <c r="O48" s="71"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="9" t="s">
@@ -6895,7 +6911,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="91"/>
+      <c r="O49" s="71"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="4" t="s">
@@ -6920,7 +6936,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="91"/>
+      <c r="O50" s="71"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="4" t="s">
@@ -6945,7 +6961,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="91"/>
+      <c r="O51" s="71"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="4" t="s">
@@ -6970,7 +6986,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="91"/>
+      <c r="O52" s="71"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="4" t="s">
@@ -6995,7 +7011,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="91"/>
+      <c r="O53" s="71"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="4" t="s">
@@ -7020,7 +7036,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="91"/>
+      <c r="O54" s="71"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="4" t="s">
@@ -7045,7 +7061,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="91"/>
+      <c r="O55" s="71"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="9" t="s">
@@ -7070,7 +7086,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="92"/>
+      <c r="O56" s="72"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="17"/>
@@ -7090,49 +7106,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="83" t="s">
+      <c r="A58" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="83"/>
-      <c r="C58" s="83"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="63"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="86" t="s">
+      <c r="F58" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="86"/>
-      <c r="H58" s="86"/>
-      <c r="I58" s="86"/>
-      <c r="J58" s="86"/>
-      <c r="K58" s="86"/>
+      <c r="G58" s="66"/>
+      <c r="H58" s="66"/>
+      <c r="I58" s="66"/>
+      <c r="J58" s="66"/>
+      <c r="K58" s="66"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="84" t="s">
+      <c r="N58" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="84"/>
+      <c r="O58" s="64"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="85"/>
-      <c r="B59" s="85"/>
-      <c r="C59" s="85"/>
+      <c r="A59" s="65"/>
+      <c r="B59" s="65"/>
+      <c r="C59" s="65"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="86"/>
-      <c r="G59" s="86"/>
-      <c r="H59" s="86"/>
-      <c r="I59" s="86"/>
-      <c r="J59" s="86"/>
-      <c r="K59" s="86"/>
+      <c r="F59" s="66"/>
+      <c r="G59" s="66"/>
+      <c r="H59" s="66"/>
+      <c r="I59" s="66"/>
+      <c r="J59" s="66"/>
+      <c r="K59" s="66"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="85"/>
-      <c r="O59" s="85"/>
+      <c r="N59" s="65"/>
+      <c r="O59" s="65"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="85"/>
-      <c r="B60" s="85"/>
-      <c r="C60" s="85"/>
+      <c r="A60" s="65"/>
+      <c r="B60" s="65"/>
+      <c r="C60" s="65"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -7143,15 +7159,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="85"/>
-      <c r="O60" s="85"/>
+      <c r="N60" s="65"/>
+      <c r="O60" s="65"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="83" t="s">
+      <c r="A61" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="83"/>
-      <c r="C61" s="83"/>
+      <c r="B61" s="63"/>
+      <c r="C61" s="63"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -7162,8 +7178,8 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="84"/>
-      <c r="O61" s="84"/>
+      <c r="N61" s="64"/>
+      <c r="O61" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="20">

</xml_diff>

<commit_message>
24.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Allocation Sheet.xlsx
+++ b/September/Others/Allocation Sheet.xlsx
@@ -433,7 +433,7 @@
     <t>V99</t>
   </si>
   <si>
-    <t>Md Robiul Islam</t>
+    <t>Md Shohel Rana</t>
   </si>
 </sst>
 </file>
@@ -806,7 +806,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -889,13 +889,93 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -950,29 +1030,44 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -985,102 +1080,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1482,7 +1481,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2582,7 +2581,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3028,7 +3027,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3099,7 +3098,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3173,7 +3172,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3244,7 +3243,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3906,8 +3905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="R55" sqref="R55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:O60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3930,50 +3929,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="55" t="s">
+      <c r="A1" s="62"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
     </row>
     <row r="3" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
       <c r="A3" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="60"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
@@ -3981,1500 +3980,1504 @@
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="M3" s="57"/>
-      <c r="N3" s="58" t="s">
+      <c r="M3" s="58"/>
+      <c r="N3" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="O3" s="59"/>
+      <c r="O3" s="60"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickTop="1">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="94" t="s">
+      <c r="D4" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="94" t="s">
+      <c r="F4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="94" t="s">
+      <c r="G4" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="94"/>
-      <c r="I4" s="93" t="s">
+      <c r="H4" s="45"/>
+      <c r="I4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="95" t="s">
+      <c r="J4" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="94" t="s">
+      <c r="K4" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="L4" s="94" t="s">
+      <c r="L4" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="M4" s="94" t="s">
+      <c r="M4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="94" t="s">
+      <c r="N4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="94" t="s">
+      <c r="O4" s="45" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A5" s="97" t="s">
+      <c r="A5" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="81">
+      <c r="B5" s="37">
         <v>800</v>
       </c>
-      <c r="C5" s="82">
+      <c r="C5" s="38">
         <v>875</v>
       </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="96" t="s">
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="J5" s="83">
+      <c r="J5" s="39">
         <v>5470</v>
       </c>
-      <c r="K5" s="82">
+      <c r="K5" s="38">
         <v>5890</v>
       </c>
-      <c r="L5" s="82"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
     </row>
     <row r="6" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="81">
+      <c r="B6" s="37">
         <v>780</v>
       </c>
-      <c r="C6" s="82">
+      <c r="C6" s="38">
         <v>840</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="96" t="s">
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="J6" s="84">
+      <c r="J6" s="40">
         <v>5750</v>
       </c>
-      <c r="K6" s="82">
+      <c r="K6" s="38">
         <v>6190</v>
       </c>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
     </row>
     <row r="7" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="81">
+      <c r="B7" s="37">
         <v>865</v>
       </c>
-      <c r="C7" s="82">
+      <c r="C7" s="38">
         <v>925</v>
       </c>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="97" t="s">
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="80">
+      <c r="J7" s="36">
         <v>5940</v>
       </c>
-      <c r="K7" s="82">
+      <c r="K7" s="38">
         <v>6390</v>
       </c>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
     </row>
     <row r="8" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A8" s="97" t="s">
+      <c r="A8" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="81">
+      <c r="B8" s="37">
         <v>810</v>
       </c>
-      <c r="C8" s="82">
+      <c r="C8" s="38">
         <v>880</v>
       </c>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="97" t="s">
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="83">
+      <c r="J8" s="39">
         <v>6530</v>
       </c>
-      <c r="K8" s="82">
+      <c r="K8" s="38">
         <v>6990</v>
       </c>
-      <c r="L8" s="82"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="82"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
     </row>
     <row r="9" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="81">
+      <c r="B9" s="37">
         <v>800</v>
       </c>
-      <c r="C9" s="82">
+      <c r="C9" s="38">
         <v>870</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="96" t="s">
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="J9" s="83">
+      <c r="J9" s="39">
         <v>6890</v>
       </c>
-      <c r="K9" s="82">
+      <c r="K9" s="38">
         <v>7490</v>
       </c>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
     </row>
     <row r="10" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A10" s="97" t="s">
+      <c r="A10" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="81">
+      <c r="B10" s="37">
         <v>795</v>
       </c>
-      <c r="C10" s="82">
+      <c r="C10" s="38">
         <v>865</v>
       </c>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="96" t="s">
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="J10" s="83">
+      <c r="J10" s="39">
         <v>8340</v>
       </c>
-      <c r="K10" s="82">
+      <c r="K10" s="38">
         <v>8990</v>
       </c>
-      <c r="L10" s="82"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="82"/>
-      <c r="O10" s="82"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
     </row>
     <row r="11" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="81">
+      <c r="B11" s="37">
         <v>790</v>
       </c>
-      <c r="C11" s="82">
+      <c r="C11" s="38">
         <v>860</v>
       </c>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="82"/>
-      <c r="I11" s="97" t="s">
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="83">
+      <c r="J11" s="39">
         <v>9190</v>
       </c>
-      <c r="K11" s="82">
+      <c r="K11" s="38">
         <v>9990</v>
       </c>
-      <c r="L11" s="82"/>
-      <c r="M11" s="82"/>
-      <c r="N11" s="82"/>
-      <c r="O11" s="82"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
     </row>
     <row r="12" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A12" s="97" t="s">
+      <c r="A12" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="B12" s="81">
+      <c r="B12" s="37">
         <v>800</v>
       </c>
-      <c r="C12" s="82">
+      <c r="C12" s="38">
         <v>860</v>
       </c>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="96" t="s">
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="J12" s="83">
+      <c r="J12" s="39">
         <v>5750</v>
       </c>
-      <c r="K12" s="82">
+      <c r="K12" s="38">
         <v>6190</v>
       </c>
-      <c r="L12" s="82"/>
-      <c r="M12" s="82"/>
-      <c r="N12" s="82"/>
-      <c r="O12" s="82"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
     </row>
     <row r="13" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="81">
+      <c r="B13" s="37">
         <v>790</v>
       </c>
-      <c r="C13" s="82">
+      <c r="C13" s="38">
         <v>850</v>
       </c>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="97" t="s">
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="J13" s="83">
+      <c r="J13" s="39">
         <v>4280</v>
       </c>
-      <c r="K13" s="82">
+      <c r="K13" s="38">
         <v>4590</v>
       </c>
-      <c r="L13" s="82"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="82"/>
-      <c r="O13" s="82"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
     </row>
     <row r="14" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="81">
+      <c r="B14" s="37">
         <v>970</v>
       </c>
-      <c r="C14" s="82">
+      <c r="C14" s="38">
         <v>1060</v>
       </c>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="82"/>
-      <c r="I14" s="96" t="s">
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="83">
+      <c r="J14" s="39">
         <v>5650</v>
       </c>
-      <c r="K14" s="82">
+      <c r="K14" s="38">
         <v>6150</v>
       </c>
-      <c r="L14" s="82"/>
-      <c r="M14" s="82"/>
-      <c r="N14" s="82"/>
-      <c r="O14" s="82"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
     </row>
     <row r="15" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="81">
+      <c r="B15" s="37">
         <v>900</v>
       </c>
-      <c r="C15" s="82">
+      <c r="C15" s="38">
         <v>975</v>
       </c>
-      <c r="D15" s="82"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="96" t="s">
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="83">
+      <c r="J15" s="39">
         <v>5020</v>
       </c>
-      <c r="K15" s="82">
+      <c r="K15" s="38">
         <v>5390</v>
       </c>
-      <c r="L15" s="82"/>
-      <c r="M15" s="82"/>
-      <c r="N15" s="82"/>
-      <c r="O15" s="82"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
     </row>
     <row r="16" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A16" s="97" t="s">
+      <c r="A16" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="81">
+      <c r="B16" s="37">
         <v>915</v>
       </c>
-      <c r="C16" s="82">
+      <c r="C16" s="38">
         <v>990</v>
       </c>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="82"/>
-      <c r="G16" s="82"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="97" t="s">
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="83">
+      <c r="J16" s="39">
         <v>5280</v>
       </c>
-      <c r="K16" s="82">
+      <c r="K16" s="38">
         <v>5690</v>
       </c>
-      <c r="L16" s="82"/>
-      <c r="M16" s="82"/>
-      <c r="N16" s="82"/>
-      <c r="O16" s="82"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
     </row>
     <row r="17" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A17" s="97" t="s">
+      <c r="A17" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="81">
+      <c r="B17" s="37">
         <v>910</v>
       </c>
-      <c r="C17" s="82">
+      <c r="C17" s="38">
         <v>980</v>
       </c>
-      <c r="D17" s="82"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="82"/>
-      <c r="G17" s="82"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="97" t="s">
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="J17" s="83">
+      <c r="J17" s="39">
         <v>4550</v>
       </c>
-      <c r="K17" s="82">
+      <c r="K17" s="38">
         <v>4890</v>
       </c>
-      <c r="L17" s="82"/>
-      <c r="M17" s="82"/>
-      <c r="N17" s="82"/>
-      <c r="O17" s="82"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
     </row>
     <row r="18" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A18" s="97" t="s">
+      <c r="A18" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="81">
+      <c r="B18" s="37">
         <v>890</v>
       </c>
-      <c r="C18" s="82">
+      <c r="C18" s="38">
         <v>970</v>
       </c>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="96" t="s">
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="J18" s="83">
+      <c r="J18" s="39">
         <v>5100</v>
       </c>
-      <c r="K18" s="82">
+      <c r="K18" s="38">
         <v>5490</v>
       </c>
-      <c r="L18" s="82"/>
-      <c r="M18" s="82"/>
-      <c r="N18" s="82"/>
-      <c r="O18" s="82"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
     </row>
     <row r="19" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A19" s="97" t="s">
+      <c r="A19" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="81">
+      <c r="B19" s="37">
         <v>920</v>
       </c>
-      <c r="C19" s="82">
+      <c r="C19" s="38">
         <v>999</v>
       </c>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="82"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="97" t="s">
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="J19" s="83">
+      <c r="J19" s="39">
         <v>5560</v>
       </c>
-      <c r="K19" s="82">
+      <c r="K19" s="38">
         <v>5990</v>
       </c>
-      <c r="L19" s="82"/>
-      <c r="M19" s="82"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="82"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
     </row>
     <row r="20" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A20" s="97" t="s">
+      <c r="A20" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="81">
+      <c r="B20" s="37">
         <v>880</v>
       </c>
-      <c r="C20" s="82">
+      <c r="C20" s="38">
         <v>950</v>
       </c>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="97" t="s">
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="83">
+      <c r="J20" s="39">
         <v>6090</v>
       </c>
-      <c r="K20" s="82">
+      <c r="K20" s="38">
         <v>6590</v>
       </c>
-      <c r="L20" s="82"/>
-      <c r="M20" s="82"/>
-      <c r="N20" s="82"/>
-      <c r="O20" s="82"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
     </row>
     <row r="21" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A21" s="97" t="s">
+      <c r="A21" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="81">
+      <c r="B21" s="37">
         <v>845</v>
       </c>
-      <c r="C21" s="82">
+      <c r="C21" s="38">
         <v>910</v>
       </c>
-      <c r="D21" s="82"/>
-      <c r="E21" s="82"/>
-      <c r="F21" s="82"/>
-      <c r="G21" s="82"/>
-      <c r="H21" s="82"/>
-      <c r="I21" s="97" t="s">
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="J21" s="83">
+      <c r="J21" s="39">
         <v>5390</v>
       </c>
-      <c r="K21" s="82">
+      <c r="K21" s="38">
         <v>5790</v>
       </c>
-      <c r="L21" s="82"/>
-      <c r="M21" s="82"/>
-      <c r="N21" s="82"/>
-      <c r="O21" s="82"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
     </row>
     <row r="22" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A22" s="97" t="s">
+      <c r="A22" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="81">
+      <c r="B22" s="37">
         <v>1000</v>
       </c>
-      <c r="C22" s="82">
+      <c r="C22" s="38">
         <v>1090</v>
       </c>
-      <c r="D22" s="82"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="82"/>
-      <c r="H22" s="82"/>
-      <c r="I22" s="97" t="s">
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="J22" s="83">
+      <c r="J22" s="39">
         <v>3630</v>
       </c>
-      <c r="K22" s="82">
+      <c r="K22" s="38">
         <v>3890</v>
       </c>
-      <c r="L22" s="82"/>
-      <c r="M22" s="82"/>
-      <c r="N22" s="82"/>
-      <c r="O22" s="82"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
     </row>
     <row r="23" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A23" s="97" t="s">
+      <c r="A23" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="81">
+      <c r="B23" s="37">
         <v>995</v>
       </c>
-      <c r="C23" s="82">
+      <c r="C23" s="38">
         <v>1075</v>
       </c>
-      <c r="D23" s="82"/>
-      <c r="E23" s="82"/>
-      <c r="F23" s="82"/>
-      <c r="G23" s="82"/>
-      <c r="H23" s="82"/>
-      <c r="I23" s="97" t="s">
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="83">
+      <c r="J23" s="39">
         <v>3560</v>
       </c>
-      <c r="K23" s="82">
+      <c r="K23" s="38">
         <v>3840</v>
       </c>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
-      <c r="N23" s="82"/>
-      <c r="O23" s="82"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
     </row>
     <row r="24" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A24" s="97" t="s">
+      <c r="A24" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="B24" s="81">
+      <c r="B24" s="37">
         <v>880</v>
       </c>
-      <c r="C24" s="82">
+      <c r="C24" s="38">
         <v>950</v>
       </c>
-      <c r="D24" s="82"/>
-      <c r="E24" s="82"/>
-      <c r="F24" s="82"/>
-      <c r="G24" s="82"/>
-      <c r="H24" s="82"/>
-      <c r="I24" s="97" t="s">
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="J24" s="83">
+      <c r="J24" s="39">
         <v>3340</v>
       </c>
-      <c r="K24" s="82">
+      <c r="K24" s="38">
         <v>3590</v>
       </c>
-      <c r="L24" s="82"/>
-      <c r="M24" s="82"/>
-      <c r="N24" s="82"/>
-      <c r="O24" s="82"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
     </row>
     <row r="25" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A25" s="97" t="s">
+      <c r="A25" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="81">
+      <c r="B25" s="37">
         <v>900</v>
       </c>
-      <c r="C25" s="82">
+      <c r="C25" s="38">
         <v>970</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="97" t="s">
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="J25" s="83">
+      <c r="J25" s="39">
         <v>5390</v>
       </c>
-      <c r="K25" s="82">
+      <c r="K25" s="38">
         <v>5790</v>
       </c>
-      <c r="L25" s="82"/>
-      <c r="M25" s="82"/>
-      <c r="N25" s="82"/>
-      <c r="O25" s="82"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
     </row>
     <row r="26" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A26" s="97" t="s">
+      <c r="A26" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="81">
+      <c r="B26" s="37">
         <v>1040</v>
       </c>
-      <c r="C26" s="82">
+      <c r="C26" s="38">
         <v>1120</v>
       </c>
-      <c r="D26" s="82"/>
-      <c r="E26" s="82"/>
-      <c r="F26" s="82"/>
-      <c r="G26" s="82"/>
-      <c r="H26" s="82"/>
-      <c r="I26" s="97" t="s">
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="J26" s="83">
+      <c r="J26" s="39">
         <v>4500</v>
       </c>
-      <c r="K26" s="82">
+      <c r="K26" s="38">
         <v>4790</v>
       </c>
-      <c r="L26" s="82"/>
-      <c r="M26" s="82"/>
-      <c r="N26" s="82"/>
-      <c r="O26" s="82"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
     </row>
     <row r="27" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A27" s="97" t="s">
+      <c r="A27" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="B27" s="81">
+      <c r="B27" s="37">
         <v>930</v>
       </c>
-      <c r="C27" s="82">
+      <c r="C27" s="38">
         <v>999</v>
       </c>
-      <c r="D27" s="82"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="82"/>
-      <c r="G27" s="82"/>
-      <c r="H27" s="82"/>
-      <c r="I27" s="96" t="s">
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="J27" s="83">
+      <c r="J27" s="39">
         <v>4970</v>
       </c>
-      <c r="K27" s="82">
+      <c r="K27" s="38">
         <v>5290</v>
       </c>
-      <c r="L27" s="82"/>
-      <c r="M27" s="82"/>
-      <c r="N27" s="82"/>
-      <c r="O27" s="82"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
     </row>
     <row r="28" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A28" s="97" t="s">
+      <c r="A28" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="81">
+      <c r="B28" s="37">
         <v>1290</v>
       </c>
-      <c r="C28" s="82">
+      <c r="C28" s="38">
         <v>1390</v>
       </c>
-      <c r="D28" s="82"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="82"/>
-      <c r="H28" s="82"/>
-      <c r="I28" s="96" t="s">
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="J28" s="83">
+      <c r="J28" s="39">
         <v>4015</v>
       </c>
-      <c r="K28" s="82">
+      <c r="K28" s="38">
         <v>4390</v>
       </c>
-      <c r="L28" s="82"/>
-      <c r="M28" s="82"/>
-      <c r="N28" s="82"/>
-      <c r="O28" s="82"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="38"/>
     </row>
     <row r="29" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A29" s="97" t="s">
+      <c r="A29" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="81">
+      <c r="B29" s="37">
         <v>1190</v>
       </c>
-      <c r="C29" s="82">
+      <c r="C29" s="38">
         <v>1290</v>
       </c>
-      <c r="D29" s="82"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="82"/>
-      <c r="G29" s="82"/>
-      <c r="H29" s="82"/>
-      <c r="I29" s="97" t="s">
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="J29" s="84">
+      <c r="J29" s="40">
         <v>3710</v>
       </c>
-      <c r="K29" s="82">
+      <c r="K29" s="38">
         <v>3990</v>
       </c>
-      <c r="L29" s="82"/>
-      <c r="M29" s="82"/>
-      <c r="N29" s="82"/>
-      <c r="O29" s="82"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
     </row>
     <row r="30" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A30" s="97" t="s">
+      <c r="A30" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="81">
+      <c r="B30" s="37">
         <v>1270</v>
       </c>
-      <c r="C30" s="82">
+      <c r="C30" s="38">
         <v>1370</v>
       </c>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="82"/>
-      <c r="G30" s="82"/>
-      <c r="H30" s="82"/>
-      <c r="I30" s="96" t="s">
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="J30" s="84">
+      <c r="J30" s="40">
         <v>3620</v>
       </c>
-      <c r="K30" s="82">
+      <c r="K30" s="38">
         <v>3890</v>
       </c>
-      <c r="L30" s="82"/>
-      <c r="M30" s="82"/>
-      <c r="N30" s="82"/>
-      <c r="O30" s="82"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
     </row>
     <row r="31" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A31" s="97" t="s">
+      <c r="A31" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="81">
+      <c r="B31" s="37">
         <v>1170</v>
       </c>
-      <c r="C31" s="82">
+      <c r="C31" s="38">
         <v>1270</v>
       </c>
-      <c r="D31" s="82"/>
-      <c r="E31" s="82"/>
-      <c r="F31" s="82"/>
-      <c r="G31" s="82"/>
-      <c r="H31" s="82"/>
-      <c r="I31" s="96" t="s">
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="84">
+      <c r="J31" s="40">
         <v>4620</v>
       </c>
-      <c r="K31" s="82">
+      <c r="K31" s="38">
         <v>4999</v>
       </c>
-      <c r="L31" s="82"/>
-      <c r="M31" s="82"/>
-      <c r="N31" s="82"/>
-      <c r="O31" s="82"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="38"/>
     </row>
     <row r="32" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A32" s="97" t="s">
+      <c r="A32" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="81">
+      <c r="B32" s="37">
         <v>1190</v>
       </c>
-      <c r="C32" s="82">
+      <c r="C32" s="38">
         <v>1290</v>
       </c>
-      <c r="D32" s="82"/>
-      <c r="E32" s="82"/>
-      <c r="F32" s="82"/>
-      <c r="G32" s="82"/>
-      <c r="H32" s="82"/>
-      <c r="I32" s="96" t="s">
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="J32" s="83">
+      <c r="J32" s="39">
         <v>4520</v>
       </c>
-      <c r="K32" s="82">
+      <c r="K32" s="38">
         <v>4899</v>
       </c>
-      <c r="L32" s="82"/>
-      <c r="M32" s="82"/>
-      <c r="N32" s="82"/>
-      <c r="O32" s="82"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="38"/>
     </row>
     <row r="33" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A33" s="97" t="s">
+      <c r="A33" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="81">
+      <c r="B33" s="37">
         <v>1225</v>
       </c>
-      <c r="C33" s="82">
+      <c r="C33" s="38">
         <v>1325</v>
       </c>
-      <c r="D33" s="82"/>
-      <c r="E33" s="82"/>
-      <c r="F33" s="82"/>
-      <c r="G33" s="82"/>
-      <c r="H33" s="82"/>
-      <c r="I33" s="97" t="s">
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="J33" s="84">
+      <c r="J33" s="40">
         <v>4080</v>
       </c>
-      <c r="K33" s="82">
+      <c r="K33" s="38">
         <v>4390</v>
       </c>
-      <c r="L33" s="82"/>
-      <c r="M33" s="82"/>
-      <c r="N33" s="82"/>
-      <c r="O33" s="82"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="38"/>
     </row>
     <row r="34" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A34" s="97" t="s">
+      <c r="A34" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="81">
+      <c r="B34" s="37">
         <v>1220</v>
       </c>
-      <c r="C34" s="82">
+      <c r="C34" s="38">
         <v>1320</v>
       </c>
-      <c r="D34" s="82"/>
-      <c r="E34" s="82"/>
-      <c r="F34" s="82"/>
-      <c r="G34" s="82"/>
-      <c r="H34" s="82"/>
-      <c r="I34" s="97" t="s">
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="J34" s="83">
+      <c r="J34" s="39">
         <v>4220</v>
       </c>
-      <c r="K34" s="82">
+      <c r="K34" s="38">
         <v>4540</v>
       </c>
-      <c r="L34" s="82"/>
-      <c r="M34" s="82"/>
-      <c r="N34" s="82"/>
-      <c r="O34" s="82"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="38"/>
     </row>
     <row r="35" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A35" s="97" t="s">
+      <c r="A35" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="85">
+      <c r="B35" s="41">
         <v>1080</v>
       </c>
-      <c r="C35" s="82">
+      <c r="C35" s="38">
         <v>1160</v>
       </c>
-      <c r="D35" s="82"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="82"/>
-      <c r="G35" s="82"/>
-      <c r="H35" s="82"/>
-      <c r="I35" s="96" t="s">
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="J35" s="83"/>
-      <c r="K35" s="82"/>
-      <c r="L35" s="82"/>
-      <c r="M35" s="82"/>
-      <c r="N35" s="82"/>
-      <c r="O35" s="82"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="38"/>
     </row>
     <row r="36" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A36" s="97" t="s">
+      <c r="A36" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="81">
+      <c r="B36" s="37">
         <v>1100</v>
       </c>
-      <c r="C36" s="82">
+      <c r="C36" s="38">
         <v>1199</v>
       </c>
-      <c r="D36" s="82"/>
-      <c r="E36" s="82"/>
-      <c r="F36" s="82"/>
-      <c r="G36" s="82"/>
-      <c r="H36" s="82"/>
-      <c r="I36" s="96" t="s">
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="J36" s="83">
+      <c r="J36" s="39">
         <v>12240</v>
       </c>
-      <c r="K36" s="82">
+      <c r="K36" s="38">
         <v>12990</v>
       </c>
-      <c r="L36" s="82"/>
-      <c r="M36" s="82"/>
-      <c r="N36" s="82"/>
-      <c r="O36" s="82"/>
+      <c r="L36" s="38"/>
+      <c r="M36" s="38"/>
+      <c r="N36" s="38"/>
+      <c r="O36" s="38"/>
     </row>
     <row r="37" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A37" s="97" t="s">
+      <c r="A37" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="81">
+      <c r="B37" s="37">
         <v>1200</v>
       </c>
-      <c r="C37" s="82">
+      <c r="C37" s="38">
         <v>1290</v>
       </c>
-      <c r="D37" s="82"/>
-      <c r="E37" s="82"/>
-      <c r="F37" s="82"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="82"/>
-      <c r="I37" s="96" t="s">
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="J37" s="83">
+      <c r="J37" s="39">
         <v>12090</v>
       </c>
-      <c r="K37" s="82">
+      <c r="K37" s="38">
         <v>12990</v>
       </c>
-      <c r="L37" s="82"/>
-      <c r="M37" s="82"/>
-      <c r="N37" s="82"/>
-      <c r="O37" s="82"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="38"/>
     </row>
     <row r="38" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A38" s="97" t="s">
+      <c r="A38" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="81">
+      <c r="B38" s="37">
         <v>1010</v>
       </c>
-      <c r="C38" s="82">
+      <c r="C38" s="38">
         <v>1110</v>
       </c>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="82"/>
-      <c r="G38" s="82"/>
-      <c r="H38" s="82"/>
-      <c r="I38" s="96" t="s">
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="J38" s="83">
+      <c r="J38" s="39">
         <v>10840</v>
       </c>
-      <c r="K38" s="82">
+      <c r="K38" s="38">
         <v>11990</v>
       </c>
-      <c r="L38" s="82"/>
-      <c r="M38" s="82"/>
-      <c r="N38" s="82"/>
-      <c r="O38" s="82"/>
+      <c r="L38" s="38"/>
+      <c r="M38" s="38"/>
+      <c r="N38" s="38"/>
+      <c r="O38" s="38"/>
     </row>
     <row r="39" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A39" s="97" t="s">
+      <c r="A39" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="81">
+      <c r="B39" s="37">
         <v>1040</v>
       </c>
-      <c r="C39" s="82">
+      <c r="C39" s="38">
         <v>1130</v>
       </c>
-      <c r="D39" s="82"/>
-      <c r="E39" s="82"/>
-      <c r="F39" s="82"/>
-      <c r="G39" s="82"/>
-      <c r="H39" s="82"/>
-      <c r="I39" s="98" t="s">
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="J39" s="84">
+      <c r="J39" s="40">
         <v>12490</v>
       </c>
-      <c r="K39" s="82">
+      <c r="K39" s="38">
         <v>13490</v>
       </c>
-      <c r="L39" s="82"/>
-      <c r="M39" s="82"/>
-      <c r="N39" s="82"/>
-      <c r="O39" s="82"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="38"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="38"/>
     </row>
     <row r="40" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A40" s="97" t="s">
+      <c r="A40" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="B40" s="81"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="82"/>
-      <c r="F40" s="82"/>
-      <c r="G40" s="82"/>
-      <c r="H40" s="82"/>
-      <c r="I40" s="96" t="s">
+      <c r="B40" s="37"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="J40" s="83">
+      <c r="J40" s="39">
         <v>8820</v>
       </c>
-      <c r="K40" s="82">
+      <c r="K40" s="38">
         <v>9490</v>
       </c>
-      <c r="L40" s="82"/>
-      <c r="M40" s="82"/>
-      <c r="N40" s="82"/>
-      <c r="O40" s="82"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="38"/>
+      <c r="N40" s="38"/>
+      <c r="O40" s="38"/>
     </row>
     <row r="41" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A41" s="97" t="s">
+      <c r="A41" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="81">
+      <c r="B41" s="37">
         <v>1100</v>
       </c>
-      <c r="C41" s="82">
+      <c r="C41" s="38">
         <v>1199</v>
       </c>
-      <c r="D41" s="82"/>
-      <c r="E41" s="82"/>
-      <c r="F41" s="82"/>
-      <c r="G41" s="82"/>
-      <c r="H41" s="82"/>
-      <c r="I41" s="96"/>
-      <c r="J41" s="83"/>
-      <c r="K41" s="82"/>
-      <c r="L41" s="82"/>
-      <c r="M41" s="82"/>
-      <c r="N41" s="82"/>
-      <c r="O41" s="82"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="47"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="38"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="38"/>
     </row>
     <row r="42" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A42" s="97" t="s">
+      <c r="A42" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="81">
+      <c r="B42" s="37">
         <v>1100</v>
       </c>
-      <c r="C42" s="82">
+      <c r="C42" s="38">
         <v>1199</v>
       </c>
-      <c r="D42" s="82"/>
-      <c r="E42" s="82"/>
-      <c r="F42" s="82"/>
-      <c r="G42" s="82"/>
-      <c r="H42" s="82"/>
-      <c r="I42" s="96"/>
-      <c r="J42" s="83"/>
-      <c r="K42" s="82"/>
-      <c r="L42" s="82"/>
-      <c r="M42" s="82"/>
-      <c r="N42" s="82"/>
-      <c r="O42" s="82"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="38"/>
+      <c r="L42" s="38"/>
+      <c r="M42" s="38"/>
+      <c r="N42" s="38"/>
+      <c r="O42" s="38"/>
     </row>
     <row r="43" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A43" s="97" t="s">
+      <c r="A43" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="81">
+      <c r="B43" s="37">
         <v>1050</v>
       </c>
-      <c r="C43" s="82">
+      <c r="C43" s="38">
         <v>1130</v>
       </c>
-      <c r="D43" s="82"/>
-      <c r="E43" s="82"/>
-      <c r="F43" s="82"/>
-      <c r="G43" s="82"/>
-      <c r="H43" s="82"/>
-      <c r="I43" s="86" t="s">
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="J43" s="86"/>
-      <c r="K43" s="82"/>
-      <c r="L43" s="82"/>
-      <c r="M43" s="86"/>
-      <c r="N43" s="86"/>
-      <c r="O43" s="87"/>
+      <c r="J43" s="50"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="50"/>
+      <c r="N43" s="50"/>
+      <c r="O43" s="42"/>
     </row>
     <row r="44" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A44" s="97" t="s">
+      <c r="A44" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="81">
+      <c r="B44" s="37">
         <v>1130</v>
       </c>
-      <c r="C44" s="82">
+      <c r="C44" s="38">
         <v>1230</v>
       </c>
-      <c r="D44" s="82"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
-      <c r="G44" s="82"/>
-      <c r="H44" s="82"/>
-      <c r="I44" s="86"/>
-      <c r="J44" s="86"/>
-      <c r="K44" s="86"/>
-      <c r="L44" s="86"/>
-      <c r="M44" s="86"/>
-      <c r="N44" s="86"/>
-      <c r="O44" s="86"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="50"/>
     </row>
     <row r="45" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A45" s="97" t="s">
+      <c r="A45" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="81">
+      <c r="B45" s="37">
         <v>1100</v>
       </c>
-      <c r="C45" s="82">
+      <c r="C45" s="38">
         <v>1190</v>
       </c>
-      <c r="D45" s="82"/>
-      <c r="E45" s="82"/>
-      <c r="F45" s="82"/>
-      <c r="G45" s="82"/>
-      <c r="H45" s="82"/>
-      <c r="I45" s="88" t="s">
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="J45" s="88"/>
-      <c r="K45" s="88"/>
-      <c r="L45" s="88"/>
-      <c r="M45" s="88"/>
-      <c r="N45" s="88"/>
-      <c r="O45" s="89"/>
+      <c r="J45" s="52"/>
+      <c r="K45" s="52"/>
+      <c r="L45" s="52"/>
+      <c r="M45" s="52"/>
+      <c r="N45" s="52"/>
+      <c r="O45" s="53"/>
     </row>
     <row r="46" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A46" s="97" t="s">
+      <c r="A46" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="81">
+      <c r="B46" s="37">
         <v>1330</v>
       </c>
-      <c r="C46" s="82">
+      <c r="C46" s="38">
         <v>1450</v>
       </c>
-      <c r="D46" s="82"/>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="82"/>
-      <c r="H46" s="82"/>
-      <c r="I46" s="82" t="s">
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="J46" s="84" t="s">
+      <c r="J46" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="K46" s="86" t="s">
+      <c r="K46" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="L46" s="86"/>
-      <c r="M46" s="86"/>
-      <c r="N46" s="86"/>
-      <c r="O46" s="90"/>
+      <c r="L46" s="50"/>
+      <c r="M46" s="50"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="54"/>
     </row>
     <row r="47" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A47" s="97" t="s">
+      <c r="A47" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="81">
+      <c r="B47" s="37">
         <v>1200</v>
       </c>
-      <c r="C47" s="82">
+      <c r="C47" s="38">
         <v>1299</v>
       </c>
-      <c r="D47" s="82"/>
-      <c r="E47" s="82"/>
-      <c r="F47" s="82"/>
-      <c r="G47" s="82"/>
-      <c r="H47" s="82"/>
-      <c r="I47" s="82">
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38">
         <v>1000</v>
       </c>
-      <c r="J47" s="84"/>
-      <c r="K47" s="82"/>
-      <c r="L47" s="82"/>
-      <c r="M47" s="82"/>
-      <c r="N47" s="82"/>
-      <c r="O47" s="90"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="38"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="38"/>
+      <c r="N47" s="38"/>
+      <c r="O47" s="54"/>
     </row>
     <row r="48" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A48" s="97" t="s">
+      <c r="A48" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="B48" s="81"/>
-      <c r="C48" s="82"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="82"/>
-      <c r="F48" s="82"/>
-      <c r="G48" s="82"/>
-      <c r="H48" s="82"/>
-      <c r="I48" s="82">
+      <c r="B48" s="37">
+        <v>1070</v>
+      </c>
+      <c r="C48" s="38">
+        <v>1160</v>
+      </c>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38">
         <v>500</v>
       </c>
-      <c r="J48" s="84"/>
-      <c r="K48" s="82"/>
-      <c r="L48" s="82"/>
-      <c r="M48" s="82"/>
-      <c r="N48" s="82"/>
-      <c r="O48" s="90"/>
+      <c r="J48" s="40"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="38"/>
+      <c r="N48" s="38"/>
+      <c r="O48" s="54"/>
     </row>
     <row r="49" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A49" s="98" t="s">
+      <c r="A49" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="82">
+      <c r="B49" s="38">
         <v>1250</v>
       </c>
-      <c r="C49" s="82">
+      <c r="C49" s="38">
         <v>1350</v>
       </c>
-      <c r="D49" s="82"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="82"/>
-      <c r="G49" s="82"/>
-      <c r="H49" s="82"/>
-      <c r="I49" s="82">
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38">
         <v>100</v>
       </c>
-      <c r="J49" s="84"/>
-      <c r="K49" s="82"/>
-      <c r="L49" s="82"/>
-      <c r="M49" s="82"/>
-      <c r="N49" s="82"/>
-      <c r="O49" s="90"/>
+      <c r="J49" s="40"/>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="38"/>
+      <c r="N49" s="38"/>
+      <c r="O49" s="54"/>
     </row>
     <row r="50" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A50" s="98" t="s">
+      <c r="A50" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="82">
+      <c r="B50" s="38">
         <v>1370</v>
       </c>
-      <c r="C50" s="82">
+      <c r="C50" s="38">
         <v>1490</v>
       </c>
-      <c r="D50" s="82"/>
-      <c r="E50" s="82"/>
-      <c r="F50" s="82"/>
-      <c r="G50" s="82"/>
-      <c r="H50" s="82"/>
-      <c r="I50" s="82">
+      <c r="D50" s="38"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38">
         <v>50</v>
       </c>
-      <c r="J50" s="84"/>
-      <c r="K50" s="82"/>
-      <c r="L50" s="82"/>
-      <c r="M50" s="82"/>
-      <c r="N50" s="82"/>
-      <c r="O50" s="90"/>
+      <c r="J50" s="40"/>
+      <c r="K50" s="38"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="38"/>
+      <c r="N50" s="38"/>
+      <c r="O50" s="54"/>
     </row>
     <row r="51" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A51" s="98" t="s">
+      <c r="A51" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="82"/>
-      <c r="C51" s="82"/>
-      <c r="D51" s="82"/>
-      <c r="E51" s="82"/>
-      <c r="F51" s="82"/>
-      <c r="G51" s="82"/>
-      <c r="H51" s="82"/>
-      <c r="I51" s="82">
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38">
         <v>20</v>
       </c>
-      <c r="J51" s="84"/>
-      <c r="K51" s="82"/>
-      <c r="L51" s="82"/>
-      <c r="M51" s="82"/>
-      <c r="N51" s="82"/>
-      <c r="O51" s="90"/>
+      <c r="J51" s="40"/>
+      <c r="K51" s="38"/>
+      <c r="L51" s="38"/>
+      <c r="M51" s="38"/>
+      <c r="N51" s="38"/>
+      <c r="O51" s="54"/>
     </row>
     <row r="52" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A52" s="98" t="s">
+      <c r="A52" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="B52" s="82">
+      <c r="B52" s="38">
         <v>1100</v>
       </c>
-      <c r="C52" s="82">
+      <c r="C52" s="38">
         <v>1190</v>
       </c>
-      <c r="D52" s="82"/>
-      <c r="E52" s="82"/>
-      <c r="F52" s="82"/>
-      <c r="G52" s="82"/>
-      <c r="H52" s="82"/>
-      <c r="I52" s="82">
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38">
         <v>10</v>
       </c>
-      <c r="J52" s="84"/>
-      <c r="K52" s="82"/>
-      <c r="L52" s="82"/>
-      <c r="M52" s="82"/>
-      <c r="N52" s="82"/>
-      <c r="O52" s="90"/>
+      <c r="J52" s="40"/>
+      <c r="K52" s="38"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="38"/>
+      <c r="N52" s="38"/>
+      <c r="O52" s="54"/>
     </row>
     <row r="53" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A53" s="98" t="s">
+      <c r="A53" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="82">
+      <c r="B53" s="38">
         <v>2780</v>
       </c>
-      <c r="C53" s="82">
+      <c r="C53" s="38">
         <v>2990</v>
       </c>
-      <c r="D53" s="82"/>
-      <c r="E53" s="82"/>
-      <c r="F53" s="82"/>
-      <c r="G53" s="82"/>
-      <c r="H53" s="82"/>
-      <c r="I53" s="82">
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38">
         <v>5</v>
       </c>
-      <c r="J53" s="84"/>
-      <c r="K53" s="82"/>
-      <c r="L53" s="82"/>
-      <c r="M53" s="82"/>
-      <c r="N53" s="82"/>
-      <c r="O53" s="90"/>
+      <c r="J53" s="40"/>
+      <c r="K53" s="38"/>
+      <c r="L53" s="38"/>
+      <c r="M53" s="38"/>
+      <c r="N53" s="38"/>
+      <c r="O53" s="54"/>
     </row>
     <row r="54" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A54" s="98" t="s">
+      <c r="A54" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="B54" s="82">
+      <c r="B54" s="38">
         <v>6540</v>
       </c>
-      <c r="C54" s="82">
+      <c r="C54" s="38">
         <v>6990</v>
       </c>
-      <c r="D54" s="82"/>
-      <c r="E54" s="82"/>
-      <c r="F54" s="82"/>
-      <c r="G54" s="82"/>
-      <c r="H54" s="82"/>
-      <c r="I54" s="82">
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38">
         <v>2</v>
       </c>
-      <c r="J54" s="84"/>
-      <c r="K54" s="82"/>
-      <c r="L54" s="82"/>
-      <c r="M54" s="82"/>
-      <c r="N54" s="82"/>
-      <c r="O54" s="90"/>
+      <c r="J54" s="40"/>
+      <c r="K54" s="38"/>
+      <c r="L54" s="38"/>
+      <c r="M54" s="38"/>
+      <c r="N54" s="38"/>
+      <c r="O54" s="54"/>
     </row>
     <row r="55" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A55" s="97" t="s">
+      <c r="A55" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B55" s="80">
+      <c r="B55" s="36">
         <v>5290</v>
       </c>
-      <c r="C55" s="80">
+      <c r="C55" s="36">
         <v>5690</v>
       </c>
-      <c r="D55" s="80"/>
-      <c r="E55" s="80"/>
-      <c r="F55" s="80"/>
-      <c r="G55" s="91"/>
-      <c r="H55" s="91"/>
-      <c r="I55" s="91" t="s">
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="43"/>
+      <c r="I55" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="J55" s="82"/>
-      <c r="K55" s="82"/>
-      <c r="L55" s="82"/>
-      <c r="M55" s="82"/>
-      <c r="N55" s="82"/>
-      <c r="O55" s="92"/>
+      <c r="J55" s="38"/>
+      <c r="K55" s="38"/>
+      <c r="L55" s="38"/>
+      <c r="M55" s="38"/>
+      <c r="N55" s="38"/>
+      <c r="O55" s="55"/>
     </row>
     <row r="56" spans="1:16">
-      <c r="A56" s="37" t="s">
+      <c r="A56" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="B56" s="38"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="41" t="s">
+      <c r="B56" s="64"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="67" t="s">
         <v>108</v>
       </c>
-      <c r="F56" s="41"/>
-      <c r="G56" s="41"/>
-      <c r="H56" s="41"/>
-      <c r="I56" s="41"/>
-      <c r="J56" s="41"/>
-      <c r="K56" s="41"/>
-      <c r="L56" s="33"/>
-      <c r="M56" s="43" t="s">
+      <c r="F56" s="67"/>
+      <c r="G56" s="67"/>
+      <c r="H56" s="67"/>
+      <c r="I56" s="67"/>
+      <c r="J56" s="67"/>
+      <c r="K56" s="67"/>
+      <c r="L56" s="32"/>
+      <c r="M56" s="69" t="s">
         <v>106</v>
       </c>
-      <c r="N56" s="43"/>
-      <c r="O56" s="44"/>
+      <c r="N56" s="69"/>
+      <c r="O56" s="70"/>
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A57" s="39"/>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="42"/>
-      <c r="F57" s="42"/>
-      <c r="G57" s="42"/>
-      <c r="H57" s="42"/>
-      <c r="I57" s="42"/>
-      <c r="J57" s="42"/>
-      <c r="K57" s="42"/>
-      <c r="L57" s="34"/>
-      <c r="M57" s="45"/>
-      <c r="N57" s="45"/>
-      <c r="O57" s="46"/>
+      <c r="A57" s="65"/>
+      <c r="B57" s="66"/>
+      <c r="C57" s="66"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="68"/>
+      <c r="F57" s="68"/>
+      <c r="G57" s="68"/>
+      <c r="H57" s="68"/>
+      <c r="I57" s="68"/>
+      <c r="J57" s="68"/>
+      <c r="K57" s="68"/>
+      <c r="L57" s="33"/>
+      <c r="M57" s="71"/>
+      <c r="N57" s="71"/>
+      <c r="O57" s="72"/>
     </row>
     <row r="58" spans="1:16">
       <c r="A58" s="29"/>
@@ -5494,50 +5497,62 @@
       <c r="O58" s="30"/>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="47" t="s">
+      <c r="A59" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="B59" s="47"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="36"/>
+      <c r="B59" s="73"/>
+      <c r="C59" s="73"/>
+      <c r="D59" s="35"/>
       <c r="E59" s="29"/>
       <c r="F59" s="29"/>
-      <c r="G59" s="49" t="s">
+      <c r="G59" s="75" t="s">
         <v>114</v>
       </c>
-      <c r="H59" s="50"/>
-      <c r="I59" s="51"/>
+      <c r="H59" s="76"/>
+      <c r="I59" s="77"/>
       <c r="J59" s="29"/>
       <c r="K59" s="29"/>
-      <c r="L59" s="36"/>
-      <c r="M59" s="48" t="s">
+      <c r="L59" s="35"/>
+      <c r="M59" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="N59" s="48"/>
-      <c r="O59" s="48"/>
+      <c r="N59" s="74"/>
+      <c r="O59" s="74"/>
     </row>
     <row r="60" spans="1:16">
-      <c r="A60" s="35"/>
-      <c r="B60" s="35"/>
-      <c r="C60" s="35"/>
-      <c r="D60" s="36"/>
+      <c r="A60" s="34"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="35"/>
       <c r="E60" s="29"/>
       <c r="F60" s="29"/>
-      <c r="G60" s="52"/>
-      <c r="H60" s="53"/>
-      <c r="I60" s="54"/>
+      <c r="G60" s="78"/>
+      <c r="H60" s="79"/>
+      <c r="I60" s="80"/>
       <c r="J60" s="29"/>
       <c r="K60" s="29"/>
-      <c r="L60" s="36"/>
+      <c r="L60" s="35"/>
       <c r="M60" s="29"/>
       <c r="N60" s="29"/>
       <c r="O60" s="29"/>
     </row>
     <row r="64" spans="1:16">
-      <c r="P64" s="32"/>
+      <c r="P64" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="E56:K57"/>
+    <mergeCell ref="M56:O57"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="M59:O59"/>
+    <mergeCell ref="G59:I60"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="I43:J43"/>
     <mergeCell ref="M43:N43"/>
     <mergeCell ref="A2:O2"/>
@@ -5545,18 +5560,6 @@
     <mergeCell ref="I45:N45"/>
     <mergeCell ref="O45:O55"/>
     <mergeCell ref="K46:N46"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="E56:K57"/>
-    <mergeCell ref="M56:O57"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="M59:O59"/>
-    <mergeCell ref="G59:I60"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.2" header="0" footer="0"/>
@@ -5593,73 +5596,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="83" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="77" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="75" t="s">
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5667,12 +5670,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="74" t="s">
+      <c r="L4" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
       <c r="A5" s="6" t="s">
@@ -6776,14 +6779,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="67" t="s">
+      <c r="I44" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="68"/>
+      <c r="J44" s="89"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="67"/>
-      <c r="N44" s="67"/>
+      <c r="M44" s="88"/>
+      <c r="N44" s="88"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -6801,13 +6804,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="67"/>
-      <c r="J45" s="67"/>
-      <c r="K45" s="67"/>
-      <c r="L45" s="67"/>
-      <c r="M45" s="67"/>
-      <c r="N45" s="67"/>
-      <c r="O45" s="67"/>
+      <c r="I45" s="88"/>
+      <c r="J45" s="88"/>
+      <c r="K45" s="88"/>
+      <c r="L45" s="88"/>
+      <c r="M45" s="88"/>
+      <c r="N45" s="88"/>
+      <c r="O45" s="88"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="9" t="s">
@@ -6824,15 +6827,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="69" t="s">
+      <c r="I46" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="69"/>
-      <c r="K46" s="69"/>
-      <c r="L46" s="69"/>
-      <c r="M46" s="69"/>
-      <c r="N46" s="69"/>
-      <c r="O46" s="70"/>
+      <c r="J46" s="90"/>
+      <c r="K46" s="90"/>
+      <c r="L46" s="90"/>
+      <c r="M46" s="90"/>
+      <c r="N46" s="90"/>
+      <c r="O46" s="91"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="9" t="s">
@@ -6855,13 +6858,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="67" t="s">
+      <c r="K47" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="67"/>
-      <c r="M47" s="67"/>
-      <c r="N47" s="67"/>
-      <c r="O47" s="71"/>
+      <c r="L47" s="88"/>
+      <c r="M47" s="88"/>
+      <c r="N47" s="88"/>
+      <c r="O47" s="92"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="9" t="s">
@@ -6886,7 +6889,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="71"/>
+      <c r="O48" s="92"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="9" t="s">
@@ -6911,7 +6914,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="71"/>
+      <c r="O49" s="92"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="4" t="s">
@@ -6936,7 +6939,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="71"/>
+      <c r="O50" s="92"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="4" t="s">
@@ -6961,7 +6964,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="71"/>
+      <c r="O51" s="92"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="4" t="s">
@@ -6986,7 +6989,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="71"/>
+      <c r="O52" s="92"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="4" t="s">
@@ -7011,7 +7014,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="71"/>
+      <c r="O53" s="92"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="4" t="s">
@@ -7036,7 +7039,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="71"/>
+      <c r="O54" s="92"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="4" t="s">
@@ -7061,7 +7064,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="71"/>
+      <c r="O55" s="92"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="9" t="s">
@@ -7086,7 +7089,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="72"/>
+      <c r="O56" s="93"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="17"/>
@@ -7106,49 +7109,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="63" t="s">
+      <c r="A58" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="63"/>
-      <c r="C58" s="63"/>
+      <c r="B58" s="94"/>
+      <c r="C58" s="94"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="66" t="s">
+      <c r="F58" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="66"/>
-      <c r="H58" s="66"/>
-      <c r="I58" s="66"/>
-      <c r="J58" s="66"/>
-      <c r="K58" s="66"/>
+      <c r="G58" s="97"/>
+      <c r="H58" s="97"/>
+      <c r="I58" s="97"/>
+      <c r="J58" s="97"/>
+      <c r="K58" s="97"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="64" t="s">
+      <c r="N58" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="64"/>
+      <c r="O58" s="95"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="65"/>
-      <c r="B59" s="65"/>
-      <c r="C59" s="65"/>
+      <c r="A59" s="96"/>
+      <c r="B59" s="96"/>
+      <c r="C59" s="96"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="66"/>
-      <c r="G59" s="66"/>
-      <c r="H59" s="66"/>
-      <c r="I59" s="66"/>
-      <c r="J59" s="66"/>
-      <c r="K59" s="66"/>
+      <c r="F59" s="97"/>
+      <c r="G59" s="97"/>
+      <c r="H59" s="97"/>
+      <c r="I59" s="97"/>
+      <c r="J59" s="97"/>
+      <c r="K59" s="97"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="65"/>
-      <c r="O59" s="65"/>
+      <c r="N59" s="96"/>
+      <c r="O59" s="96"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="65"/>
-      <c r="B60" s="65"/>
-      <c r="C60" s="65"/>
+      <c r="A60" s="96"/>
+      <c r="B60" s="96"/>
+      <c r="C60" s="96"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -7159,15 +7162,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="65"/>
-      <c r="O60" s="65"/>
+      <c r="N60" s="96"/>
+      <c r="O60" s="96"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="63" t="s">
+      <c r="A61" s="94" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="63"/>
-      <c r="C61" s="63"/>
+      <c r="B61" s="94"/>
+      <c r="C61" s="94"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -7178,11 +7181,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="64"/>
-      <c r="O61" s="64"/>
+      <c r="N61" s="95"/>
+      <c r="O61" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="A59:C60"/>
+    <mergeCell ref="N59:O60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="F58:K59"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="A1:E1"/>
@@ -7190,19 +7206,6 @@
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="A59:C60"/>
-    <mergeCell ref="N59:O60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="F58:K59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>